<commit_message>
Finalized OrangeHRM QA testing project with bug reports and screenshots
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -135,6 +135,25 @@
     <t>Medium</t>
   </si>
   <si>
+    <t>Log005</t>
+  </si>
+  <si>
+    <t>redirects after log out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login 
+2. Logout
+3. Click back button in browser.  
+4. Click on any tab ("Admin", "PIM", "Leave", ...)
+5. Login with different user  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard for new user should be display. </t>
+  </si>
+  <si>
+    <t>❌ Redirects to previous clicked tab from user that was login in before</t>
+  </si>
+  <si>
     <t>Admin001</t>
   </si>
   <si>
@@ -158,13 +177,86 @@
     <t>Admin002</t>
   </si>
   <si>
+    <t>Add existing user. Check from another tab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to Admin tab
+2. Go to User Management
+3. Add new user
+4. Go to a new browser tab  
+5. Go to admin.
+6. Check if user was added. </t>
+  </si>
+  <si>
+    <t>User is added to records</t>
+  </si>
+  <si>
+    <t>Admin003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete User. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to Admin tab
+2. Go to User Management
+3. Click on delete user
+4. Delete user </t>
+  </si>
+  <si>
+    <t>Success message should be display. User should be remove of records</t>
+  </si>
+  <si>
+    <t>Admin004</t>
+  </si>
+  <si>
+    <t>Search username by partial or incomplete username</t>
+  </si>
+  <si>
+    <t>1. Go to Admin tab &gt; User Management
+2. In the username search field, type only part of a existing name. 
+3. Click search.</t>
+  </si>
+  <si>
+    <t>The system returns all users that match the partial input (e.g., all usernames that start with or contain the letters entered)</t>
+  </si>
+  <si>
+    <t>❌ Search fails unless the full exact username is entered</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Pim001</t>
+  </si>
+  <si>
+    <t>PIM</t>
+  </si>
+  <si>
+    <t>SQL Injection-Like Behavior in Employee ID Search Field Returns All Records</t>
+  </si>
+  <si>
+    <t>1. Go to PIM &gt; Employee List
+2. In the Employee ID field, enter ' OR 1=1 --
+3. Click Search
+4. Observe the result</t>
+  </si>
+  <si>
+    <t>App should sanitize input. No server error should occur. Should never exposed all records when filter is malformed,</t>
+  </si>
+  <si>
+    <t>❌ Backend returns a 422 error in Network Tab. 123 records all still shown.</t>
+  </si>
+  <si>
+    <t>Medium to High</t>
+  </si>
+  <si>
     <t>Leave001</t>
   </si>
   <si>
     <t>Leave tab</t>
   </si>
   <si>
-    <t>Navingating to leave tab after login in</t>
+    <t>Navigating to leave tab after login in</t>
   </si>
   <si>
     <t>1. login
@@ -226,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -269,7 +361,17 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -493,11 +595,12 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="10.5"/>
     <col customWidth="1" min="2" max="2" width="8.38"/>
-    <col customWidth="1" min="3" max="3" width="32.38"/>
+    <col customWidth="1" min="3" max="3" width="58.5"/>
     <col customWidth="1" min="4" max="4" width="51.0"/>
-    <col customWidth="1" min="5" max="5" width="50.38"/>
+    <col customWidth="1" min="5" max="5" width="89.75"/>
     <col customWidth="1" min="6" max="6" width="60.63"/>
     <col customWidth="1" min="7" max="7" width="8.63"/>
+    <col customWidth="1" min="8" max="8" width="13.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -631,32 +734,47 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="14"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>13</v>
@@ -669,3009 +787,3105 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="15"/>
+      <c r="A8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="13" t="s">
+      <c r="C9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="D10" s="15"/>
+      <c r="H10" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="11">
-      <c r="D11" s="15"/>
+      <c r="A11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12">
-      <c r="D12" s="15"/>
+      <c r="A12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="13">
-      <c r="D13" s="15"/>
+      <c r="D13" s="19"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14">
-      <c r="D14" s="15"/>
+      <c r="D14" s="19"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15">
-      <c r="D15" s="15"/>
+      <c r="D15" s="19"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16">
-      <c r="D16" s="15"/>
+      <c r="D16" s="19"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17">
-      <c r="D17" s="15"/>
+      <c r="D17" s="19"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18">
-      <c r="D18" s="15"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19">
-      <c r="D19" s="15"/>
+      <c r="D19" s="19"/>
     </row>
     <row r="20">
-      <c r="D20" s="15"/>
+      <c r="D20" s="19"/>
     </row>
     <row r="21">
-      <c r="D21" s="15"/>
+      <c r="D21" s="19"/>
     </row>
     <row r="22">
-      <c r="D22" s="15"/>
+      <c r="D22" s="19"/>
     </row>
     <row r="23">
-      <c r="D23" s="15"/>
+      <c r="D23" s="19"/>
     </row>
     <row r="24">
-      <c r="D24" s="15"/>
+      <c r="D24" s="19"/>
     </row>
     <row r="25">
-      <c r="D25" s="15"/>
+      <c r="D25" s="19"/>
     </row>
     <row r="26">
-      <c r="D26" s="15"/>
+      <c r="D26" s="19"/>
     </row>
     <row r="27">
-      <c r="D27" s="15"/>
+      <c r="D27" s="19"/>
     </row>
     <row r="28">
-      <c r="D28" s="15"/>
+      <c r="D28" s="19"/>
     </row>
     <row r="29">
-      <c r="D29" s="15"/>
+      <c r="D29" s="19"/>
     </row>
     <row r="30">
-      <c r="D30" s="15"/>
+      <c r="D30" s="19"/>
     </row>
     <row r="31">
-      <c r="D31" s="15"/>
+      <c r="D31" s="19"/>
     </row>
     <row r="32">
-      <c r="D32" s="15"/>
+      <c r="D32" s="19"/>
     </row>
     <row r="33">
-      <c r="D33" s="15"/>
+      <c r="D33" s="19"/>
     </row>
     <row r="34">
-      <c r="D34" s="15"/>
+      <c r="D34" s="19"/>
     </row>
     <row r="35">
-      <c r="D35" s="15"/>
+      <c r="D35" s="19"/>
     </row>
     <row r="36">
-      <c r="D36" s="15"/>
+      <c r="D36" s="19"/>
     </row>
     <row r="37">
-      <c r="D37" s="15"/>
+      <c r="D37" s="19"/>
     </row>
     <row r="38">
-      <c r="D38" s="15"/>
+      <c r="D38" s="19"/>
     </row>
     <row r="39">
-      <c r="D39" s="15"/>
+      <c r="D39" s="19"/>
     </row>
     <row r="40">
-      <c r="D40" s="15"/>
+      <c r="D40" s="19"/>
     </row>
     <row r="41">
-      <c r="D41" s="15"/>
+      <c r="D41" s="19"/>
     </row>
     <row r="42">
-      <c r="D42" s="15"/>
+      <c r="D42" s="19"/>
     </row>
     <row r="43">
-      <c r="D43" s="15"/>
+      <c r="D43" s="19"/>
     </row>
     <row r="44">
-      <c r="D44" s="15"/>
+      <c r="D44" s="19"/>
     </row>
     <row r="45">
-      <c r="D45" s="15"/>
+      <c r="D45" s="19"/>
     </row>
     <row r="46">
-      <c r="D46" s="15"/>
+      <c r="D46" s="19"/>
     </row>
     <row r="47">
-      <c r="D47" s="15"/>
+      <c r="D47" s="19"/>
     </row>
     <row r="48">
-      <c r="D48" s="15"/>
+      <c r="D48" s="19"/>
     </row>
     <row r="49">
-      <c r="D49" s="15"/>
+      <c r="D49" s="19"/>
     </row>
     <row r="50">
-      <c r="D50" s="15"/>
+      <c r="D50" s="19"/>
     </row>
     <row r="51">
-      <c r="D51" s="15"/>
+      <c r="D51" s="19"/>
     </row>
     <row r="52">
-      <c r="D52" s="15"/>
+      <c r="D52" s="19"/>
     </row>
     <row r="53">
-      <c r="D53" s="15"/>
+      <c r="D53" s="19"/>
     </row>
     <row r="54">
-      <c r="D54" s="15"/>
+      <c r="D54" s="19"/>
     </row>
     <row r="55">
-      <c r="D55" s="15"/>
+      <c r="D55" s="19"/>
     </row>
     <row r="56">
-      <c r="D56" s="15"/>
+      <c r="D56" s="19"/>
     </row>
     <row r="57">
-      <c r="D57" s="15"/>
+      <c r="D57" s="19"/>
     </row>
     <row r="58">
-      <c r="D58" s="15"/>
+      <c r="D58" s="19"/>
     </row>
     <row r="59">
-      <c r="D59" s="15"/>
+      <c r="D59" s="19"/>
     </row>
     <row r="60">
-      <c r="D60" s="15"/>
+      <c r="D60" s="19"/>
     </row>
     <row r="61">
-      <c r="D61" s="15"/>
+      <c r="D61" s="19"/>
     </row>
     <row r="62">
-      <c r="D62" s="15"/>
+      <c r="D62" s="19"/>
     </row>
     <row r="63">
-      <c r="D63" s="15"/>
+      <c r="D63" s="19"/>
     </row>
     <row r="64">
-      <c r="D64" s="15"/>
+      <c r="D64" s="19"/>
     </row>
     <row r="65">
-      <c r="D65" s="15"/>
+      <c r="D65" s="19"/>
     </row>
     <row r="66">
-      <c r="D66" s="15"/>
+      <c r="D66" s="19"/>
     </row>
     <row r="67">
-      <c r="D67" s="15"/>
+      <c r="D67" s="19"/>
     </row>
     <row r="68">
-      <c r="D68" s="15"/>
+      <c r="D68" s="19"/>
     </row>
     <row r="69">
-      <c r="D69" s="15"/>
+      <c r="D69" s="19"/>
     </row>
     <row r="70">
-      <c r="D70" s="15"/>
+      <c r="D70" s="19"/>
     </row>
     <row r="71">
-      <c r="D71" s="15"/>
+      <c r="D71" s="19"/>
     </row>
     <row r="72">
-      <c r="D72" s="15"/>
+      <c r="D72" s="19"/>
     </row>
     <row r="73">
-      <c r="D73" s="15"/>
+      <c r="D73" s="19"/>
     </row>
     <row r="74">
-      <c r="D74" s="15"/>
+      <c r="D74" s="19"/>
     </row>
     <row r="75">
-      <c r="D75" s="15"/>
+      <c r="D75" s="19"/>
     </row>
     <row r="76">
-      <c r="D76" s="15"/>
+      <c r="D76" s="19"/>
     </row>
     <row r="77">
-      <c r="D77" s="15"/>
+      <c r="D77" s="19"/>
     </row>
     <row r="78">
-      <c r="D78" s="15"/>
+      <c r="D78" s="19"/>
     </row>
     <row r="79">
-      <c r="D79" s="15"/>
+      <c r="D79" s="19"/>
     </row>
     <row r="80">
-      <c r="D80" s="15"/>
+      <c r="D80" s="19"/>
     </row>
     <row r="81">
-      <c r="D81" s="15"/>
+      <c r="D81" s="19"/>
     </row>
     <row r="82">
-      <c r="D82" s="15"/>
+      <c r="D82" s="19"/>
     </row>
     <row r="83">
-      <c r="D83" s="15"/>
+      <c r="D83" s="19"/>
     </row>
     <row r="84">
-      <c r="D84" s="15"/>
+      <c r="D84" s="19"/>
     </row>
     <row r="85">
-      <c r="D85" s="15"/>
+      <c r="D85" s="19"/>
     </row>
     <row r="86">
-      <c r="D86" s="15"/>
+      <c r="D86" s="19"/>
     </row>
     <row r="87">
-      <c r="D87" s="15"/>
+      <c r="D87" s="19"/>
     </row>
     <row r="88">
-      <c r="D88" s="15"/>
+      <c r="D88" s="19"/>
     </row>
     <row r="89">
-      <c r="D89" s="15"/>
+      <c r="D89" s="19"/>
     </row>
     <row r="90">
-      <c r="D90" s="15"/>
+      <c r="D90" s="19"/>
     </row>
     <row r="91">
-      <c r="D91" s="15"/>
+      <c r="D91" s="19"/>
     </row>
     <row r="92">
-      <c r="D92" s="15"/>
+      <c r="D92" s="19"/>
     </row>
     <row r="93">
-      <c r="D93" s="15"/>
+      <c r="D93" s="19"/>
     </row>
     <row r="94">
-      <c r="D94" s="15"/>
+      <c r="D94" s="19"/>
     </row>
     <row r="95">
-      <c r="D95" s="15"/>
+      <c r="D95" s="19"/>
     </row>
     <row r="96">
-      <c r="D96" s="15"/>
+      <c r="D96" s="19"/>
     </row>
     <row r="97">
-      <c r="D97" s="15"/>
+      <c r="D97" s="19"/>
     </row>
     <row r="98">
-      <c r="D98" s="15"/>
+      <c r="D98" s="19"/>
     </row>
     <row r="99">
-      <c r="D99" s="15"/>
+      <c r="D99" s="19"/>
     </row>
     <row r="100">
-      <c r="D100" s="15"/>
+      <c r="D100" s="19"/>
     </row>
     <row r="101">
-      <c r="D101" s="15"/>
+      <c r="D101" s="19"/>
     </row>
     <row r="102">
-      <c r="D102" s="15"/>
+      <c r="D102" s="19"/>
     </row>
     <row r="103">
-      <c r="D103" s="15"/>
+      <c r="D103" s="19"/>
     </row>
     <row r="104">
-      <c r="D104" s="15"/>
+      <c r="D104" s="19"/>
     </row>
     <row r="105">
-      <c r="D105" s="15"/>
+      <c r="D105" s="19"/>
     </row>
     <row r="106">
-      <c r="D106" s="15"/>
+      <c r="D106" s="19"/>
     </row>
     <row r="107">
-      <c r="D107" s="15"/>
+      <c r="D107" s="19"/>
     </row>
     <row r="108">
-      <c r="D108" s="15"/>
+      <c r="D108" s="19"/>
     </row>
     <row r="109">
-      <c r="D109" s="15"/>
+      <c r="D109" s="19"/>
     </row>
     <row r="110">
-      <c r="D110" s="15"/>
+      <c r="D110" s="19"/>
     </row>
     <row r="111">
-      <c r="D111" s="15"/>
+      <c r="D111" s="19"/>
     </row>
     <row r="112">
-      <c r="D112" s="15"/>
+      <c r="D112" s="19"/>
     </row>
     <row r="113">
-      <c r="D113" s="15"/>
+      <c r="D113" s="19"/>
     </row>
     <row r="114">
-      <c r="D114" s="15"/>
+      <c r="D114" s="19"/>
     </row>
     <row r="115">
-      <c r="D115" s="15"/>
+      <c r="D115" s="19"/>
     </row>
     <row r="116">
-      <c r="D116" s="15"/>
+      <c r="D116" s="19"/>
     </row>
     <row r="117">
-      <c r="D117" s="15"/>
+      <c r="D117" s="19"/>
     </row>
     <row r="118">
-      <c r="D118" s="15"/>
+      <c r="D118" s="19"/>
     </row>
     <row r="119">
-      <c r="D119" s="15"/>
+      <c r="D119" s="19"/>
     </row>
     <row r="120">
-      <c r="D120" s="15"/>
+      <c r="D120" s="19"/>
     </row>
     <row r="121">
-      <c r="D121" s="15"/>
+      <c r="D121" s="19"/>
     </row>
     <row r="122">
-      <c r="D122" s="15"/>
+      <c r="D122" s="19"/>
     </row>
     <row r="123">
-      <c r="D123" s="15"/>
+      <c r="D123" s="19"/>
     </row>
     <row r="124">
-      <c r="D124" s="15"/>
+      <c r="D124" s="19"/>
     </row>
     <row r="125">
-      <c r="D125" s="15"/>
+      <c r="D125" s="19"/>
     </row>
     <row r="126">
-      <c r="D126" s="15"/>
+      <c r="D126" s="19"/>
     </row>
     <row r="127">
-      <c r="D127" s="15"/>
+      <c r="D127" s="19"/>
     </row>
     <row r="128">
-      <c r="D128" s="15"/>
+      <c r="D128" s="19"/>
     </row>
     <row r="129">
-      <c r="D129" s="15"/>
+      <c r="D129" s="19"/>
     </row>
     <row r="130">
-      <c r="D130" s="15"/>
+      <c r="D130" s="19"/>
     </row>
     <row r="131">
-      <c r="D131" s="15"/>
+      <c r="D131" s="19"/>
     </row>
     <row r="132">
-      <c r="D132" s="15"/>
+      <c r="D132" s="19"/>
     </row>
     <row r="133">
-      <c r="D133" s="15"/>
+      <c r="D133" s="19"/>
     </row>
     <row r="134">
-      <c r="D134" s="15"/>
+      <c r="D134" s="19"/>
     </row>
     <row r="135">
-      <c r="D135" s="15"/>
+      <c r="D135" s="19"/>
     </row>
     <row r="136">
-      <c r="D136" s="15"/>
+      <c r="D136" s="19"/>
     </row>
     <row r="137">
-      <c r="D137" s="15"/>
+      <c r="D137" s="19"/>
     </row>
     <row r="138">
-      <c r="D138" s="15"/>
+      <c r="D138" s="19"/>
     </row>
     <row r="139">
-      <c r="D139" s="15"/>
+      <c r="D139" s="19"/>
     </row>
     <row r="140">
-      <c r="D140" s="15"/>
+      <c r="D140" s="19"/>
     </row>
     <row r="141">
-      <c r="D141" s="15"/>
+      <c r="D141" s="19"/>
     </row>
     <row r="142">
-      <c r="D142" s="15"/>
+      <c r="D142" s="19"/>
     </row>
     <row r="143">
-      <c r="D143" s="15"/>
+      <c r="D143" s="19"/>
     </row>
     <row r="144">
-      <c r="D144" s="15"/>
+      <c r="D144" s="19"/>
     </row>
     <row r="145">
-      <c r="D145" s="15"/>
+      <c r="D145" s="19"/>
     </row>
     <row r="146">
-      <c r="D146" s="15"/>
+      <c r="D146" s="19"/>
     </row>
     <row r="147">
-      <c r="D147" s="15"/>
+      <c r="D147" s="19"/>
     </row>
     <row r="148">
-      <c r="D148" s="15"/>
+      <c r="D148" s="19"/>
     </row>
     <row r="149">
-      <c r="D149" s="15"/>
+      <c r="D149" s="19"/>
     </row>
     <row r="150">
-      <c r="D150" s="15"/>
+      <c r="D150" s="19"/>
     </row>
     <row r="151">
-      <c r="D151" s="15"/>
+      <c r="D151" s="19"/>
     </row>
     <row r="152">
-      <c r="D152" s="15"/>
+      <c r="D152" s="19"/>
     </row>
     <row r="153">
-      <c r="D153" s="15"/>
+      <c r="D153" s="19"/>
     </row>
     <row r="154">
-      <c r="D154" s="15"/>
+      <c r="D154" s="19"/>
     </row>
     <row r="155">
-      <c r="D155" s="15"/>
+      <c r="D155" s="19"/>
     </row>
     <row r="156">
-      <c r="D156" s="15"/>
+      <c r="D156" s="19"/>
     </row>
     <row r="157">
-      <c r="D157" s="15"/>
+      <c r="D157" s="19"/>
     </row>
     <row r="158">
-      <c r="D158" s="15"/>
+      <c r="D158" s="19"/>
     </row>
     <row r="159">
-      <c r="D159" s="15"/>
+      <c r="D159" s="19"/>
     </row>
     <row r="160">
-      <c r="D160" s="15"/>
+      <c r="D160" s="19"/>
     </row>
     <row r="161">
-      <c r="D161" s="15"/>
+      <c r="D161" s="19"/>
     </row>
     <row r="162">
-      <c r="D162" s="15"/>
+      <c r="D162" s="19"/>
     </row>
     <row r="163">
-      <c r="D163" s="15"/>
+      <c r="D163" s="19"/>
     </row>
     <row r="164">
-      <c r="D164" s="15"/>
+      <c r="D164" s="19"/>
     </row>
     <row r="165">
-      <c r="D165" s="15"/>
+      <c r="D165" s="19"/>
     </row>
     <row r="166">
-      <c r="D166" s="15"/>
+      <c r="D166" s="19"/>
     </row>
     <row r="167">
-      <c r="D167" s="15"/>
+      <c r="D167" s="19"/>
     </row>
     <row r="168">
-      <c r="D168" s="15"/>
+      <c r="D168" s="19"/>
     </row>
     <row r="169">
-      <c r="D169" s="15"/>
+      <c r="D169" s="19"/>
     </row>
     <row r="170">
-      <c r="D170" s="15"/>
+      <c r="D170" s="19"/>
     </row>
     <row r="171">
-      <c r="D171" s="15"/>
+      <c r="D171" s="19"/>
     </row>
     <row r="172">
-      <c r="D172" s="15"/>
+      <c r="D172" s="19"/>
     </row>
     <row r="173">
-      <c r="D173" s="15"/>
+      <c r="D173" s="19"/>
     </row>
     <row r="174">
-      <c r="D174" s="15"/>
+      <c r="D174" s="19"/>
     </row>
     <row r="175">
-      <c r="D175" s="15"/>
+      <c r="D175" s="19"/>
     </row>
     <row r="176">
-      <c r="D176" s="15"/>
+      <c r="D176" s="19"/>
     </row>
     <row r="177">
-      <c r="D177" s="15"/>
+      <c r="D177" s="19"/>
     </row>
     <row r="178">
-      <c r="D178" s="15"/>
+      <c r="D178" s="19"/>
     </row>
     <row r="179">
-      <c r="D179" s="15"/>
+      <c r="D179" s="19"/>
     </row>
     <row r="180">
-      <c r="D180" s="15"/>
+      <c r="D180" s="19"/>
     </row>
     <row r="181">
-      <c r="D181" s="15"/>
+      <c r="D181" s="19"/>
     </row>
     <row r="182">
-      <c r="D182" s="15"/>
+      <c r="D182" s="19"/>
     </row>
     <row r="183">
-      <c r="D183" s="15"/>
+      <c r="D183" s="19"/>
     </row>
     <row r="184">
-      <c r="D184" s="15"/>
+      <c r="D184" s="19"/>
     </row>
     <row r="185">
-      <c r="D185" s="15"/>
+      <c r="D185" s="19"/>
     </row>
     <row r="186">
-      <c r="D186" s="15"/>
+      <c r="D186" s="19"/>
     </row>
     <row r="187">
-      <c r="D187" s="15"/>
+      <c r="D187" s="19"/>
     </row>
     <row r="188">
-      <c r="D188" s="15"/>
+      <c r="D188" s="19"/>
     </row>
     <row r="189">
-      <c r="D189" s="15"/>
+      <c r="D189" s="19"/>
     </row>
     <row r="190">
-      <c r="D190" s="15"/>
+      <c r="D190" s="19"/>
     </row>
     <row r="191">
-      <c r="D191" s="15"/>
+      <c r="D191" s="19"/>
     </row>
     <row r="192">
-      <c r="D192" s="15"/>
+      <c r="D192" s="19"/>
     </row>
     <row r="193">
-      <c r="D193" s="15"/>
+      <c r="D193" s="19"/>
     </row>
     <row r="194">
-      <c r="D194" s="15"/>
+      <c r="D194" s="19"/>
     </row>
     <row r="195">
-      <c r="D195" s="15"/>
+      <c r="D195" s="19"/>
     </row>
     <row r="196">
-      <c r="D196" s="15"/>
+      <c r="D196" s="19"/>
     </row>
     <row r="197">
-      <c r="D197" s="15"/>
+      <c r="D197" s="19"/>
     </row>
     <row r="198">
-      <c r="D198" s="15"/>
+      <c r="D198" s="19"/>
     </row>
     <row r="199">
-      <c r="D199" s="15"/>
+      <c r="D199" s="19"/>
     </row>
     <row r="200">
-      <c r="D200" s="15"/>
+      <c r="D200" s="19"/>
     </row>
     <row r="201">
-      <c r="D201" s="15"/>
+      <c r="D201" s="19"/>
     </row>
     <row r="202">
-      <c r="D202" s="15"/>
+      <c r="D202" s="19"/>
     </row>
     <row r="203">
-      <c r="D203" s="15"/>
+      <c r="D203" s="19"/>
     </row>
     <row r="204">
-      <c r="D204" s="15"/>
+      <c r="D204" s="19"/>
     </row>
     <row r="205">
-      <c r="D205" s="15"/>
+      <c r="D205" s="19"/>
     </row>
     <row r="206">
-      <c r="D206" s="15"/>
+      <c r="D206" s="19"/>
     </row>
     <row r="207">
-      <c r="D207" s="15"/>
+      <c r="D207" s="19"/>
     </row>
     <row r="208">
-      <c r="D208" s="15"/>
+      <c r="D208" s="19"/>
     </row>
     <row r="209">
-      <c r="D209" s="15"/>
+      <c r="D209" s="19"/>
     </row>
     <row r="210">
-      <c r="D210" s="15"/>
+      <c r="D210" s="19"/>
     </row>
     <row r="211">
-      <c r="D211" s="15"/>
+      <c r="D211" s="19"/>
     </row>
     <row r="212">
-      <c r="D212" s="15"/>
+      <c r="D212" s="19"/>
     </row>
     <row r="213">
-      <c r="D213" s="15"/>
+      <c r="D213" s="19"/>
     </row>
     <row r="214">
-      <c r="D214" s="15"/>
+      <c r="D214" s="19"/>
     </row>
     <row r="215">
-      <c r="D215" s="15"/>
+      <c r="D215" s="19"/>
     </row>
     <row r="216">
-      <c r="D216" s="15"/>
+      <c r="D216" s="19"/>
     </row>
     <row r="217">
-      <c r="D217" s="15"/>
+      <c r="D217" s="19"/>
     </row>
     <row r="218">
-      <c r="D218" s="15"/>
+      <c r="D218" s="19"/>
     </row>
     <row r="219">
-      <c r="D219" s="15"/>
+      <c r="D219" s="19"/>
     </row>
     <row r="220">
-      <c r="D220" s="15"/>
+      <c r="D220" s="19"/>
     </row>
     <row r="221">
-      <c r="D221" s="15"/>
+      <c r="D221" s="19"/>
     </row>
     <row r="222">
-      <c r="D222" s="15"/>
+      <c r="D222" s="19"/>
     </row>
     <row r="223">
-      <c r="D223" s="15"/>
+      <c r="D223" s="19"/>
     </row>
     <row r="224">
-      <c r="D224" s="15"/>
+      <c r="D224" s="19"/>
     </row>
     <row r="225">
-      <c r="D225" s="15"/>
+      <c r="D225" s="19"/>
     </row>
     <row r="226">
-      <c r="D226" s="15"/>
+      <c r="D226" s="19"/>
     </row>
     <row r="227">
-      <c r="D227" s="15"/>
+      <c r="D227" s="19"/>
     </row>
     <row r="228">
-      <c r="D228" s="15"/>
+      <c r="D228" s="19"/>
     </row>
     <row r="229">
-      <c r="D229" s="15"/>
+      <c r="D229" s="19"/>
     </row>
     <row r="230">
-      <c r="D230" s="15"/>
+      <c r="D230" s="19"/>
     </row>
     <row r="231">
-      <c r="D231" s="15"/>
+      <c r="D231" s="19"/>
     </row>
     <row r="232">
-      <c r="D232" s="15"/>
+      <c r="D232" s="19"/>
     </row>
     <row r="233">
-      <c r="D233" s="15"/>
+      <c r="D233" s="19"/>
     </row>
     <row r="234">
-      <c r="D234" s="15"/>
+      <c r="D234" s="19"/>
     </row>
     <row r="235">
-      <c r="D235" s="15"/>
+      <c r="D235" s="19"/>
     </row>
     <row r="236">
-      <c r="D236" s="15"/>
+      <c r="D236" s="19"/>
     </row>
     <row r="237">
-      <c r="D237" s="15"/>
+      <c r="D237" s="19"/>
     </row>
     <row r="238">
-      <c r="D238" s="15"/>
+      <c r="D238" s="19"/>
     </row>
     <row r="239">
-      <c r="D239" s="15"/>
+      <c r="D239" s="19"/>
     </row>
     <row r="240">
-      <c r="D240" s="15"/>
+      <c r="D240" s="19"/>
     </row>
     <row r="241">
-      <c r="D241" s="15"/>
+      <c r="D241" s="19"/>
     </row>
     <row r="242">
-      <c r="D242" s="15"/>
+      <c r="D242" s="19"/>
     </row>
     <row r="243">
-      <c r="D243" s="15"/>
+      <c r="D243" s="19"/>
     </row>
     <row r="244">
-      <c r="D244" s="15"/>
+      <c r="D244" s="19"/>
     </row>
     <row r="245">
-      <c r="D245" s="15"/>
+      <c r="D245" s="19"/>
     </row>
     <row r="246">
-      <c r="D246" s="15"/>
+      <c r="D246" s="19"/>
     </row>
     <row r="247">
-      <c r="D247" s="15"/>
+      <c r="D247" s="19"/>
     </row>
     <row r="248">
-      <c r="D248" s="15"/>
+      <c r="D248" s="19"/>
     </row>
     <row r="249">
-      <c r="D249" s="15"/>
+      <c r="D249" s="19"/>
     </row>
     <row r="250">
-      <c r="D250" s="15"/>
+      <c r="D250" s="19"/>
     </row>
     <row r="251">
-      <c r="D251" s="15"/>
+      <c r="D251" s="19"/>
     </row>
     <row r="252">
-      <c r="D252" s="15"/>
+      <c r="D252" s="19"/>
     </row>
     <row r="253">
-      <c r="D253" s="15"/>
+      <c r="D253" s="19"/>
     </row>
     <row r="254">
-      <c r="D254" s="15"/>
+      <c r="D254" s="19"/>
     </row>
     <row r="255">
-      <c r="D255" s="15"/>
+      <c r="D255" s="19"/>
     </row>
     <row r="256">
-      <c r="D256" s="15"/>
+      <c r="D256" s="19"/>
     </row>
     <row r="257">
-      <c r="D257" s="15"/>
+      <c r="D257" s="19"/>
     </row>
     <row r="258">
-      <c r="D258" s="15"/>
+      <c r="D258" s="19"/>
     </row>
     <row r="259">
-      <c r="D259" s="15"/>
+      <c r="D259" s="19"/>
     </row>
     <row r="260">
-      <c r="D260" s="15"/>
+      <c r="D260" s="19"/>
     </row>
     <row r="261">
-      <c r="D261" s="15"/>
+      <c r="D261" s="19"/>
     </row>
     <row r="262">
-      <c r="D262" s="15"/>
+      <c r="D262" s="19"/>
     </row>
     <row r="263">
-      <c r="D263" s="15"/>
+      <c r="D263" s="19"/>
     </row>
     <row r="264">
-      <c r="D264" s="15"/>
+      <c r="D264" s="19"/>
     </row>
     <row r="265">
-      <c r="D265" s="15"/>
+      <c r="D265" s="19"/>
     </row>
     <row r="266">
-      <c r="D266" s="15"/>
+      <c r="D266" s="19"/>
     </row>
     <row r="267">
-      <c r="D267" s="15"/>
+      <c r="D267" s="19"/>
     </row>
     <row r="268">
-      <c r="D268" s="15"/>
+      <c r="D268" s="19"/>
     </row>
     <row r="269">
-      <c r="D269" s="15"/>
+      <c r="D269" s="19"/>
     </row>
     <row r="270">
-      <c r="D270" s="15"/>
+      <c r="D270" s="19"/>
     </row>
     <row r="271">
-      <c r="D271" s="15"/>
+      <c r="D271" s="19"/>
     </row>
     <row r="272">
-      <c r="D272" s="15"/>
+      <c r="D272" s="19"/>
     </row>
     <row r="273">
-      <c r="D273" s="15"/>
+      <c r="D273" s="19"/>
     </row>
     <row r="274">
-      <c r="D274" s="15"/>
+      <c r="D274" s="19"/>
     </row>
     <row r="275">
-      <c r="D275" s="15"/>
+      <c r="D275" s="19"/>
     </row>
     <row r="276">
-      <c r="D276" s="15"/>
+      <c r="D276" s="19"/>
     </row>
     <row r="277">
-      <c r="D277" s="15"/>
+      <c r="D277" s="19"/>
     </row>
     <row r="278">
-      <c r="D278" s="15"/>
+      <c r="D278" s="19"/>
     </row>
     <row r="279">
-      <c r="D279" s="15"/>
+      <c r="D279" s="19"/>
     </row>
     <row r="280">
-      <c r="D280" s="15"/>
+      <c r="D280" s="19"/>
     </row>
     <row r="281">
-      <c r="D281" s="15"/>
+      <c r="D281" s="19"/>
     </row>
     <row r="282">
-      <c r="D282" s="15"/>
+      <c r="D282" s="19"/>
     </row>
     <row r="283">
-      <c r="D283" s="15"/>
+      <c r="D283" s="19"/>
     </row>
     <row r="284">
-      <c r="D284" s="15"/>
+      <c r="D284" s="19"/>
     </row>
     <row r="285">
-      <c r="D285" s="15"/>
+      <c r="D285" s="19"/>
     </row>
     <row r="286">
-      <c r="D286" s="15"/>
+      <c r="D286" s="19"/>
     </row>
     <row r="287">
-      <c r="D287" s="15"/>
+      <c r="D287" s="19"/>
     </row>
     <row r="288">
-      <c r="D288" s="15"/>
+      <c r="D288" s="19"/>
     </row>
     <row r="289">
-      <c r="D289" s="15"/>
+      <c r="D289" s="19"/>
     </row>
     <row r="290">
-      <c r="D290" s="15"/>
+      <c r="D290" s="19"/>
     </row>
     <row r="291">
-      <c r="D291" s="15"/>
+      <c r="D291" s="19"/>
     </row>
     <row r="292">
-      <c r="D292" s="15"/>
+      <c r="D292" s="19"/>
     </row>
     <row r="293">
-      <c r="D293" s="15"/>
+      <c r="D293" s="19"/>
     </row>
     <row r="294">
-      <c r="D294" s="15"/>
+      <c r="D294" s="19"/>
     </row>
     <row r="295">
-      <c r="D295" s="15"/>
+      <c r="D295" s="19"/>
     </row>
     <row r="296">
-      <c r="D296" s="15"/>
+      <c r="D296" s="19"/>
     </row>
     <row r="297">
-      <c r="D297" s="15"/>
+      <c r="D297" s="19"/>
     </row>
     <row r="298">
-      <c r="D298" s="15"/>
+      <c r="D298" s="19"/>
     </row>
     <row r="299">
-      <c r="D299" s="15"/>
+      <c r="D299" s="19"/>
     </row>
     <row r="300">
-      <c r="D300" s="15"/>
+      <c r="D300" s="19"/>
     </row>
     <row r="301">
-      <c r="D301" s="15"/>
+      <c r="D301" s="19"/>
     </row>
     <row r="302">
-      <c r="D302" s="15"/>
+      <c r="D302" s="19"/>
     </row>
     <row r="303">
-      <c r="D303" s="15"/>
+      <c r="D303" s="19"/>
     </row>
     <row r="304">
-      <c r="D304" s="15"/>
+      <c r="D304" s="19"/>
     </row>
     <row r="305">
-      <c r="D305" s="15"/>
+      <c r="D305" s="19"/>
     </row>
     <row r="306">
-      <c r="D306" s="15"/>
+      <c r="D306" s="19"/>
     </row>
     <row r="307">
-      <c r="D307" s="15"/>
+      <c r="D307" s="19"/>
     </row>
     <row r="308">
-      <c r="D308" s="15"/>
+      <c r="D308" s="19"/>
     </row>
     <row r="309">
-      <c r="D309" s="15"/>
+      <c r="D309" s="19"/>
     </row>
     <row r="310">
-      <c r="D310" s="15"/>
+      <c r="D310" s="19"/>
     </row>
     <row r="311">
-      <c r="D311" s="15"/>
+      <c r="D311" s="19"/>
     </row>
     <row r="312">
-      <c r="D312" s="15"/>
+      <c r="D312" s="19"/>
     </row>
     <row r="313">
-      <c r="D313" s="15"/>
+      <c r="D313" s="19"/>
     </row>
     <row r="314">
-      <c r="D314" s="15"/>
+      <c r="D314" s="19"/>
     </row>
     <row r="315">
-      <c r="D315" s="15"/>
+      <c r="D315" s="19"/>
     </row>
     <row r="316">
-      <c r="D316" s="15"/>
+      <c r="D316" s="19"/>
     </row>
     <row r="317">
-      <c r="D317" s="15"/>
+      <c r="D317" s="19"/>
     </row>
     <row r="318">
-      <c r="D318" s="15"/>
+      <c r="D318" s="19"/>
     </row>
     <row r="319">
-      <c r="D319" s="15"/>
+      <c r="D319" s="19"/>
     </row>
     <row r="320">
-      <c r="D320" s="15"/>
+      <c r="D320" s="19"/>
     </row>
     <row r="321">
-      <c r="D321" s="15"/>
+      <c r="D321" s="19"/>
     </row>
     <row r="322">
-      <c r="D322" s="15"/>
+      <c r="D322" s="19"/>
     </row>
     <row r="323">
-      <c r="D323" s="15"/>
+      <c r="D323" s="19"/>
     </row>
     <row r="324">
-      <c r="D324" s="15"/>
+      <c r="D324" s="19"/>
     </row>
     <row r="325">
-      <c r="D325" s="15"/>
+      <c r="D325" s="19"/>
     </row>
     <row r="326">
-      <c r="D326" s="15"/>
+      <c r="D326" s="19"/>
     </row>
     <row r="327">
-      <c r="D327" s="15"/>
+      <c r="D327" s="19"/>
     </row>
     <row r="328">
-      <c r="D328" s="15"/>
+      <c r="D328" s="19"/>
     </row>
     <row r="329">
-      <c r="D329" s="15"/>
+      <c r="D329" s="19"/>
     </row>
     <row r="330">
-      <c r="D330" s="15"/>
+      <c r="D330" s="19"/>
     </row>
     <row r="331">
-      <c r="D331" s="15"/>
+      <c r="D331" s="19"/>
     </row>
     <row r="332">
-      <c r="D332" s="15"/>
+      <c r="D332" s="19"/>
     </row>
     <row r="333">
-      <c r="D333" s="15"/>
+      <c r="D333" s="19"/>
     </row>
     <row r="334">
-      <c r="D334" s="15"/>
+      <c r="D334" s="19"/>
     </row>
     <row r="335">
-      <c r="D335" s="15"/>
+      <c r="D335" s="19"/>
     </row>
     <row r="336">
-      <c r="D336" s="15"/>
+      <c r="D336" s="19"/>
     </row>
     <row r="337">
-      <c r="D337" s="15"/>
+      <c r="D337" s="19"/>
     </row>
     <row r="338">
-      <c r="D338" s="15"/>
+      <c r="D338" s="19"/>
     </row>
     <row r="339">
-      <c r="D339" s="15"/>
+      <c r="D339" s="19"/>
     </row>
     <row r="340">
-      <c r="D340" s="15"/>
+      <c r="D340" s="19"/>
     </row>
     <row r="341">
-      <c r="D341" s="15"/>
+      <c r="D341" s="19"/>
     </row>
     <row r="342">
-      <c r="D342" s="15"/>
+      <c r="D342" s="19"/>
     </row>
     <row r="343">
-      <c r="D343" s="15"/>
+      <c r="D343" s="19"/>
     </row>
     <row r="344">
-      <c r="D344" s="15"/>
+      <c r="D344" s="19"/>
     </row>
     <row r="345">
-      <c r="D345" s="15"/>
+      <c r="D345" s="19"/>
     </row>
     <row r="346">
-      <c r="D346" s="15"/>
+      <c r="D346" s="19"/>
     </row>
     <row r="347">
-      <c r="D347" s="15"/>
+      <c r="D347" s="19"/>
     </row>
     <row r="348">
-      <c r="D348" s="15"/>
+      <c r="D348" s="19"/>
     </row>
     <row r="349">
-      <c r="D349" s="15"/>
+      <c r="D349" s="19"/>
     </row>
     <row r="350">
-      <c r="D350" s="15"/>
+      <c r="D350" s="19"/>
     </row>
     <row r="351">
-      <c r="D351" s="15"/>
+      <c r="D351" s="19"/>
     </row>
     <row r="352">
-      <c r="D352" s="15"/>
+      <c r="D352" s="19"/>
     </row>
     <row r="353">
-      <c r="D353" s="15"/>
+      <c r="D353" s="19"/>
     </row>
     <row r="354">
-      <c r="D354" s="15"/>
+      <c r="D354" s="19"/>
     </row>
     <row r="355">
-      <c r="D355" s="15"/>
+      <c r="D355" s="19"/>
     </row>
     <row r="356">
-      <c r="D356" s="15"/>
+      <c r="D356" s="19"/>
     </row>
     <row r="357">
-      <c r="D357" s="15"/>
+      <c r="D357" s="19"/>
     </row>
     <row r="358">
-      <c r="D358" s="15"/>
+      <c r="D358" s="19"/>
     </row>
     <row r="359">
-      <c r="D359" s="15"/>
+      <c r="D359" s="19"/>
     </row>
     <row r="360">
-      <c r="D360" s="15"/>
+      <c r="D360" s="19"/>
     </row>
     <row r="361">
-      <c r="D361" s="15"/>
+      <c r="D361" s="19"/>
     </row>
     <row r="362">
-      <c r="D362" s="15"/>
+      <c r="D362" s="19"/>
     </row>
     <row r="363">
-      <c r="D363" s="15"/>
+      <c r="D363" s="19"/>
     </row>
     <row r="364">
-      <c r="D364" s="15"/>
+      <c r="D364" s="19"/>
     </row>
     <row r="365">
-      <c r="D365" s="15"/>
+      <c r="D365" s="19"/>
     </row>
     <row r="366">
-      <c r="D366" s="15"/>
+      <c r="D366" s="19"/>
     </row>
     <row r="367">
-      <c r="D367" s="15"/>
+      <c r="D367" s="19"/>
     </row>
     <row r="368">
-      <c r="D368" s="15"/>
+      <c r="D368" s="19"/>
     </row>
     <row r="369">
-      <c r="D369" s="15"/>
+      <c r="D369" s="19"/>
     </row>
     <row r="370">
-      <c r="D370" s="15"/>
+      <c r="D370" s="19"/>
     </row>
     <row r="371">
-      <c r="D371" s="15"/>
+      <c r="D371" s="19"/>
     </row>
     <row r="372">
-      <c r="D372" s="15"/>
+      <c r="D372" s="19"/>
     </row>
     <row r="373">
-      <c r="D373" s="15"/>
+      <c r="D373" s="19"/>
     </row>
     <row r="374">
-      <c r="D374" s="15"/>
+      <c r="D374" s="19"/>
     </row>
     <row r="375">
-      <c r="D375" s="15"/>
+      <c r="D375" s="19"/>
     </row>
     <row r="376">
-      <c r="D376" s="15"/>
+      <c r="D376" s="19"/>
     </row>
     <row r="377">
-      <c r="D377" s="15"/>
+      <c r="D377" s="19"/>
     </row>
     <row r="378">
-      <c r="D378" s="15"/>
+      <c r="D378" s="19"/>
     </row>
     <row r="379">
-      <c r="D379" s="15"/>
+      <c r="D379" s="19"/>
     </row>
     <row r="380">
-      <c r="D380" s="15"/>
+      <c r="D380" s="19"/>
     </row>
     <row r="381">
-      <c r="D381" s="15"/>
+      <c r="D381" s="19"/>
     </row>
     <row r="382">
-      <c r="D382" s="15"/>
+      <c r="D382" s="19"/>
     </row>
     <row r="383">
-      <c r="D383" s="15"/>
+      <c r="D383" s="19"/>
     </row>
     <row r="384">
-      <c r="D384" s="15"/>
+      <c r="D384" s="19"/>
     </row>
     <row r="385">
-      <c r="D385" s="15"/>
+      <c r="D385" s="19"/>
     </row>
     <row r="386">
-      <c r="D386" s="15"/>
+      <c r="D386" s="19"/>
     </row>
     <row r="387">
-      <c r="D387" s="15"/>
+      <c r="D387" s="19"/>
     </row>
     <row r="388">
-      <c r="D388" s="15"/>
+      <c r="D388" s="19"/>
     </row>
     <row r="389">
-      <c r="D389" s="15"/>
+      <c r="D389" s="19"/>
     </row>
     <row r="390">
-      <c r="D390" s="15"/>
+      <c r="D390" s="19"/>
     </row>
     <row r="391">
-      <c r="D391" s="15"/>
+      <c r="D391" s="19"/>
     </row>
     <row r="392">
-      <c r="D392" s="15"/>
+      <c r="D392" s="19"/>
     </row>
     <row r="393">
-      <c r="D393" s="15"/>
+      <c r="D393" s="19"/>
     </row>
     <row r="394">
-      <c r="D394" s="15"/>
+      <c r="D394" s="19"/>
     </row>
     <row r="395">
-      <c r="D395" s="15"/>
+      <c r="D395" s="19"/>
     </row>
     <row r="396">
-      <c r="D396" s="15"/>
+      <c r="D396" s="19"/>
     </row>
     <row r="397">
-      <c r="D397" s="15"/>
+      <c r="D397" s="19"/>
     </row>
     <row r="398">
-      <c r="D398" s="15"/>
+      <c r="D398" s="19"/>
     </row>
     <row r="399">
-      <c r="D399" s="15"/>
+      <c r="D399" s="19"/>
     </row>
     <row r="400">
-      <c r="D400" s="15"/>
+      <c r="D400" s="19"/>
     </row>
     <row r="401">
-      <c r="D401" s="15"/>
+      <c r="D401" s="19"/>
     </row>
     <row r="402">
-      <c r="D402" s="15"/>
+      <c r="D402" s="19"/>
     </row>
     <row r="403">
-      <c r="D403" s="15"/>
+      <c r="D403" s="19"/>
     </row>
     <row r="404">
-      <c r="D404" s="15"/>
+      <c r="D404" s="19"/>
     </row>
     <row r="405">
-      <c r="D405" s="15"/>
+      <c r="D405" s="19"/>
     </row>
     <row r="406">
-      <c r="D406" s="15"/>
+      <c r="D406" s="19"/>
     </row>
     <row r="407">
-      <c r="D407" s="15"/>
+      <c r="D407" s="19"/>
     </row>
     <row r="408">
-      <c r="D408" s="15"/>
+      <c r="D408" s="19"/>
     </row>
     <row r="409">
-      <c r="D409" s="15"/>
+      <c r="D409" s="19"/>
     </row>
     <row r="410">
-      <c r="D410" s="15"/>
+      <c r="D410" s="19"/>
     </row>
     <row r="411">
-      <c r="D411" s="15"/>
+      <c r="D411" s="19"/>
     </row>
     <row r="412">
-      <c r="D412" s="15"/>
+      <c r="D412" s="19"/>
     </row>
     <row r="413">
-      <c r="D413" s="15"/>
+      <c r="D413" s="19"/>
     </row>
     <row r="414">
-      <c r="D414" s="15"/>
+      <c r="D414" s="19"/>
     </row>
     <row r="415">
-      <c r="D415" s="15"/>
+      <c r="D415" s="19"/>
     </row>
     <row r="416">
-      <c r="D416" s="15"/>
+      <c r="D416" s="19"/>
     </row>
     <row r="417">
-      <c r="D417" s="15"/>
+      <c r="D417" s="19"/>
     </row>
     <row r="418">
-      <c r="D418" s="15"/>
+      <c r="D418" s="19"/>
     </row>
     <row r="419">
-      <c r="D419" s="15"/>
+      <c r="D419" s="19"/>
     </row>
     <row r="420">
-      <c r="D420" s="15"/>
+      <c r="D420" s="19"/>
     </row>
     <row r="421">
-      <c r="D421" s="15"/>
+      <c r="D421" s="19"/>
     </row>
     <row r="422">
-      <c r="D422" s="15"/>
+      <c r="D422" s="19"/>
     </row>
     <row r="423">
-      <c r="D423" s="15"/>
+      <c r="D423" s="19"/>
     </row>
     <row r="424">
-      <c r="D424" s="15"/>
+      <c r="D424" s="19"/>
     </row>
     <row r="425">
-      <c r="D425" s="15"/>
+      <c r="D425" s="19"/>
     </row>
     <row r="426">
-      <c r="D426" s="15"/>
+      <c r="D426" s="19"/>
     </row>
     <row r="427">
-      <c r="D427" s="15"/>
+      <c r="D427" s="19"/>
     </row>
     <row r="428">
-      <c r="D428" s="15"/>
+      <c r="D428" s="19"/>
     </row>
     <row r="429">
-      <c r="D429" s="15"/>
+      <c r="D429" s="19"/>
     </row>
     <row r="430">
-      <c r="D430" s="15"/>
+      <c r="D430" s="19"/>
     </row>
     <row r="431">
-      <c r="D431" s="15"/>
+      <c r="D431" s="19"/>
     </row>
     <row r="432">
-      <c r="D432" s="15"/>
+      <c r="D432" s="19"/>
     </row>
     <row r="433">
-      <c r="D433" s="15"/>
+      <c r="D433" s="19"/>
     </row>
     <row r="434">
-      <c r="D434" s="15"/>
+      <c r="D434" s="19"/>
     </row>
     <row r="435">
-      <c r="D435" s="15"/>
+      <c r="D435" s="19"/>
     </row>
     <row r="436">
-      <c r="D436" s="15"/>
+      <c r="D436" s="19"/>
     </row>
     <row r="437">
-      <c r="D437" s="15"/>
+      <c r="D437" s="19"/>
     </row>
     <row r="438">
-      <c r="D438" s="15"/>
+      <c r="D438" s="19"/>
     </row>
     <row r="439">
-      <c r="D439" s="15"/>
+      <c r="D439" s="19"/>
     </row>
     <row r="440">
-      <c r="D440" s="15"/>
+      <c r="D440" s="19"/>
     </row>
     <row r="441">
-      <c r="D441" s="15"/>
+      <c r="D441" s="19"/>
     </row>
     <row r="442">
-      <c r="D442" s="15"/>
+      <c r="D442" s="19"/>
     </row>
     <row r="443">
-      <c r="D443" s="15"/>
+      <c r="D443" s="19"/>
     </row>
     <row r="444">
-      <c r="D444" s="15"/>
+      <c r="D444" s="19"/>
     </row>
     <row r="445">
-      <c r="D445" s="15"/>
+      <c r="D445" s="19"/>
     </row>
     <row r="446">
-      <c r="D446" s="15"/>
+      <c r="D446" s="19"/>
     </row>
     <row r="447">
-      <c r="D447" s="15"/>
+      <c r="D447" s="19"/>
     </row>
     <row r="448">
-      <c r="D448" s="15"/>
+      <c r="D448" s="19"/>
     </row>
     <row r="449">
-      <c r="D449" s="15"/>
+      <c r="D449" s="19"/>
     </row>
     <row r="450">
-      <c r="D450" s="15"/>
+      <c r="D450" s="19"/>
     </row>
     <row r="451">
-      <c r="D451" s="15"/>
+      <c r="D451" s="19"/>
     </row>
     <row r="452">
-      <c r="D452" s="15"/>
+      <c r="D452" s="19"/>
     </row>
     <row r="453">
-      <c r="D453" s="15"/>
+      <c r="D453" s="19"/>
     </row>
     <row r="454">
-      <c r="D454" s="15"/>
+      <c r="D454" s="19"/>
     </row>
     <row r="455">
-      <c r="D455" s="15"/>
+      <c r="D455" s="19"/>
     </row>
     <row r="456">
-      <c r="D456" s="15"/>
+      <c r="D456" s="19"/>
     </row>
     <row r="457">
-      <c r="D457" s="15"/>
+      <c r="D457" s="19"/>
     </row>
     <row r="458">
-      <c r="D458" s="15"/>
+      <c r="D458" s="19"/>
     </row>
     <row r="459">
-      <c r="D459" s="15"/>
+      <c r="D459" s="19"/>
     </row>
     <row r="460">
-      <c r="D460" s="15"/>
+      <c r="D460" s="19"/>
     </row>
     <row r="461">
-      <c r="D461" s="15"/>
+      <c r="D461" s="19"/>
     </row>
     <row r="462">
-      <c r="D462" s="15"/>
+      <c r="D462" s="19"/>
     </row>
     <row r="463">
-      <c r="D463" s="15"/>
+      <c r="D463" s="19"/>
     </row>
     <row r="464">
-      <c r="D464" s="15"/>
+      <c r="D464" s="19"/>
     </row>
     <row r="465">
-      <c r="D465" s="15"/>
+      <c r="D465" s="19"/>
     </row>
     <row r="466">
-      <c r="D466" s="15"/>
+      <c r="D466" s="19"/>
     </row>
     <row r="467">
-      <c r="D467" s="15"/>
+      <c r="D467" s="19"/>
     </row>
     <row r="468">
-      <c r="D468" s="15"/>
+      <c r="D468" s="19"/>
     </row>
     <row r="469">
-      <c r="D469" s="15"/>
+      <c r="D469" s="19"/>
     </row>
     <row r="470">
-      <c r="D470" s="15"/>
+      <c r="D470" s="19"/>
     </row>
     <row r="471">
-      <c r="D471" s="15"/>
+      <c r="D471" s="19"/>
     </row>
     <row r="472">
-      <c r="D472" s="15"/>
+      <c r="D472" s="19"/>
     </row>
     <row r="473">
-      <c r="D473" s="15"/>
+      <c r="D473" s="19"/>
     </row>
     <row r="474">
-      <c r="D474" s="15"/>
+      <c r="D474" s="19"/>
     </row>
     <row r="475">
-      <c r="D475" s="15"/>
+      <c r="D475" s="19"/>
     </row>
     <row r="476">
-      <c r="D476" s="15"/>
+      <c r="D476" s="19"/>
     </row>
     <row r="477">
-      <c r="D477" s="15"/>
+      <c r="D477" s="19"/>
     </row>
     <row r="478">
-      <c r="D478" s="15"/>
+      <c r="D478" s="19"/>
     </row>
     <row r="479">
-      <c r="D479" s="15"/>
+      <c r="D479" s="19"/>
     </row>
     <row r="480">
-      <c r="D480" s="15"/>
+      <c r="D480" s="19"/>
     </row>
     <row r="481">
-      <c r="D481" s="15"/>
+      <c r="D481" s="19"/>
     </row>
     <row r="482">
-      <c r="D482" s="15"/>
+      <c r="D482" s="19"/>
     </row>
     <row r="483">
-      <c r="D483" s="15"/>
+      <c r="D483" s="19"/>
     </row>
     <row r="484">
-      <c r="D484" s="15"/>
+      <c r="D484" s="19"/>
     </row>
     <row r="485">
-      <c r="D485" s="15"/>
+      <c r="D485" s="19"/>
     </row>
     <row r="486">
-      <c r="D486" s="15"/>
+      <c r="D486" s="19"/>
     </row>
     <row r="487">
-      <c r="D487" s="15"/>
+      <c r="D487" s="19"/>
     </row>
     <row r="488">
-      <c r="D488" s="15"/>
+      <c r="D488" s="19"/>
     </row>
     <row r="489">
-      <c r="D489" s="15"/>
+      <c r="D489" s="19"/>
     </row>
     <row r="490">
-      <c r="D490" s="15"/>
+      <c r="D490" s="19"/>
     </row>
     <row r="491">
-      <c r="D491" s="15"/>
+      <c r="D491" s="19"/>
     </row>
     <row r="492">
-      <c r="D492" s="15"/>
+      <c r="D492" s="19"/>
     </row>
     <row r="493">
-      <c r="D493" s="15"/>
+      <c r="D493" s="19"/>
     </row>
     <row r="494">
-      <c r="D494" s="15"/>
+      <c r="D494" s="19"/>
     </row>
     <row r="495">
-      <c r="D495" s="15"/>
+      <c r="D495" s="19"/>
     </row>
     <row r="496">
-      <c r="D496" s="15"/>
+      <c r="D496" s="19"/>
     </row>
     <row r="497">
-      <c r="D497" s="15"/>
+      <c r="D497" s="19"/>
     </row>
     <row r="498">
-      <c r="D498" s="15"/>
+      <c r="D498" s="19"/>
     </row>
     <row r="499">
-      <c r="D499" s="15"/>
+      <c r="D499" s="19"/>
     </row>
     <row r="500">
-      <c r="D500" s="15"/>
+      <c r="D500" s="19"/>
     </row>
     <row r="501">
-      <c r="D501" s="15"/>
+      <c r="D501" s="19"/>
     </row>
     <row r="502">
-      <c r="D502" s="15"/>
+      <c r="D502" s="19"/>
     </row>
     <row r="503">
-      <c r="D503" s="15"/>
+      <c r="D503" s="19"/>
     </row>
     <row r="504">
-      <c r="D504" s="15"/>
+      <c r="D504" s="19"/>
     </row>
     <row r="505">
-      <c r="D505" s="15"/>
+      <c r="D505" s="19"/>
     </row>
     <row r="506">
-      <c r="D506" s="15"/>
+      <c r="D506" s="19"/>
     </row>
     <row r="507">
-      <c r="D507" s="15"/>
+      <c r="D507" s="19"/>
     </row>
     <row r="508">
-      <c r="D508" s="15"/>
+      <c r="D508" s="19"/>
     </row>
     <row r="509">
-      <c r="D509" s="15"/>
+      <c r="D509" s="19"/>
     </row>
     <row r="510">
-      <c r="D510" s="15"/>
+      <c r="D510" s="19"/>
     </row>
     <row r="511">
-      <c r="D511" s="15"/>
+      <c r="D511" s="19"/>
     </row>
     <row r="512">
-      <c r="D512" s="15"/>
+      <c r="D512" s="19"/>
     </row>
     <row r="513">
-      <c r="D513" s="15"/>
+      <c r="D513" s="19"/>
     </row>
     <row r="514">
-      <c r="D514" s="15"/>
+      <c r="D514" s="19"/>
     </row>
     <row r="515">
-      <c r="D515" s="15"/>
+      <c r="D515" s="19"/>
     </row>
     <row r="516">
-      <c r="D516" s="15"/>
+      <c r="D516" s="19"/>
     </row>
     <row r="517">
-      <c r="D517" s="15"/>
+      <c r="D517" s="19"/>
     </row>
     <row r="518">
-      <c r="D518" s="15"/>
+      <c r="D518" s="19"/>
     </row>
     <row r="519">
-      <c r="D519" s="15"/>
+      <c r="D519" s="19"/>
     </row>
     <row r="520">
-      <c r="D520" s="15"/>
+      <c r="D520" s="19"/>
     </row>
     <row r="521">
-      <c r="D521" s="15"/>
+      <c r="D521" s="19"/>
     </row>
     <row r="522">
-      <c r="D522" s="15"/>
+      <c r="D522" s="19"/>
     </row>
     <row r="523">
-      <c r="D523" s="15"/>
+      <c r="D523" s="19"/>
     </row>
     <row r="524">
-      <c r="D524" s="15"/>
+      <c r="D524" s="19"/>
     </row>
     <row r="525">
-      <c r="D525" s="15"/>
+      <c r="D525" s="19"/>
     </row>
     <row r="526">
-      <c r="D526" s="15"/>
+      <c r="D526" s="19"/>
     </row>
     <row r="527">
-      <c r="D527" s="15"/>
+      <c r="D527" s="19"/>
     </row>
     <row r="528">
-      <c r="D528" s="15"/>
+      <c r="D528" s="19"/>
     </row>
     <row r="529">
-      <c r="D529" s="15"/>
+      <c r="D529" s="19"/>
     </row>
     <row r="530">
-      <c r="D530" s="15"/>
+      <c r="D530" s="19"/>
     </row>
     <row r="531">
-      <c r="D531" s="15"/>
+      <c r="D531" s="19"/>
     </row>
     <row r="532">
-      <c r="D532" s="15"/>
+      <c r="D532" s="19"/>
     </row>
     <row r="533">
-      <c r="D533" s="15"/>
+      <c r="D533" s="19"/>
     </row>
     <row r="534">
-      <c r="D534" s="15"/>
+      <c r="D534" s="19"/>
     </row>
     <row r="535">
-      <c r="D535" s="15"/>
+      <c r="D535" s="19"/>
     </row>
     <row r="536">
-      <c r="D536" s="15"/>
+      <c r="D536" s="19"/>
     </row>
     <row r="537">
-      <c r="D537" s="15"/>
+      <c r="D537" s="19"/>
     </row>
     <row r="538">
-      <c r="D538" s="15"/>
+      <c r="D538" s="19"/>
     </row>
     <row r="539">
-      <c r="D539" s="15"/>
+      <c r="D539" s="19"/>
     </row>
     <row r="540">
-      <c r="D540" s="15"/>
+      <c r="D540" s="19"/>
     </row>
     <row r="541">
-      <c r="D541" s="15"/>
+      <c r="D541" s="19"/>
     </row>
     <row r="542">
-      <c r="D542" s="15"/>
+      <c r="D542" s="19"/>
     </row>
     <row r="543">
-      <c r="D543" s="15"/>
+      <c r="D543" s="19"/>
     </row>
     <row r="544">
-      <c r="D544" s="15"/>
+      <c r="D544" s="19"/>
     </row>
     <row r="545">
-      <c r="D545" s="15"/>
+      <c r="D545" s="19"/>
     </row>
     <row r="546">
-      <c r="D546" s="15"/>
+      <c r="D546" s="19"/>
     </row>
     <row r="547">
-      <c r="D547" s="15"/>
+      <c r="D547" s="19"/>
     </row>
     <row r="548">
-      <c r="D548" s="15"/>
+      <c r="D548" s="19"/>
     </row>
     <row r="549">
-      <c r="D549" s="15"/>
+      <c r="D549" s="19"/>
     </row>
     <row r="550">
-      <c r="D550" s="15"/>
+      <c r="D550" s="19"/>
     </row>
     <row r="551">
-      <c r="D551" s="15"/>
+      <c r="D551" s="19"/>
     </row>
     <row r="552">
-      <c r="D552" s="15"/>
+      <c r="D552" s="19"/>
     </row>
     <row r="553">
-      <c r="D553" s="15"/>
+      <c r="D553" s="19"/>
     </row>
     <row r="554">
-      <c r="D554" s="15"/>
+      <c r="D554" s="19"/>
     </row>
     <row r="555">
-      <c r="D555" s="15"/>
+      <c r="D555" s="19"/>
     </row>
     <row r="556">
-      <c r="D556" s="15"/>
+      <c r="D556" s="19"/>
     </row>
     <row r="557">
-      <c r="D557" s="15"/>
+      <c r="D557" s="19"/>
     </row>
     <row r="558">
-      <c r="D558" s="15"/>
+      <c r="D558" s="19"/>
     </row>
     <row r="559">
-      <c r="D559" s="15"/>
+      <c r="D559" s="19"/>
     </row>
     <row r="560">
-      <c r="D560" s="15"/>
+      <c r="D560" s="19"/>
     </row>
     <row r="561">
-      <c r="D561" s="15"/>
+      <c r="D561" s="19"/>
     </row>
     <row r="562">
-      <c r="D562" s="15"/>
+      <c r="D562" s="19"/>
     </row>
     <row r="563">
-      <c r="D563" s="15"/>
+      <c r="D563" s="19"/>
     </row>
     <row r="564">
-      <c r="D564" s="15"/>
+      <c r="D564" s="19"/>
     </row>
     <row r="565">
-      <c r="D565" s="15"/>
+      <c r="D565" s="19"/>
     </row>
     <row r="566">
-      <c r="D566" s="15"/>
+      <c r="D566" s="19"/>
     </row>
     <row r="567">
-      <c r="D567" s="15"/>
+      <c r="D567" s="19"/>
     </row>
     <row r="568">
-      <c r="D568" s="15"/>
+      <c r="D568" s="19"/>
     </row>
     <row r="569">
-      <c r="D569" s="15"/>
+      <c r="D569" s="19"/>
     </row>
     <row r="570">
-      <c r="D570" s="15"/>
+      <c r="D570" s="19"/>
     </row>
     <row r="571">
-      <c r="D571" s="15"/>
+      <c r="D571" s="19"/>
     </row>
     <row r="572">
-      <c r="D572" s="15"/>
+      <c r="D572" s="19"/>
     </row>
     <row r="573">
-      <c r="D573" s="15"/>
+      <c r="D573" s="19"/>
     </row>
     <row r="574">
-      <c r="D574" s="15"/>
+      <c r="D574" s="19"/>
     </row>
     <row r="575">
-      <c r="D575" s="15"/>
+      <c r="D575" s="19"/>
     </row>
     <row r="576">
-      <c r="D576" s="15"/>
+      <c r="D576" s="19"/>
     </row>
     <row r="577">
-      <c r="D577" s="15"/>
+      <c r="D577" s="19"/>
     </row>
     <row r="578">
-      <c r="D578" s="15"/>
+      <c r="D578" s="19"/>
     </row>
     <row r="579">
-      <c r="D579" s="15"/>
+      <c r="D579" s="19"/>
     </row>
     <row r="580">
-      <c r="D580" s="15"/>
+      <c r="D580" s="19"/>
     </row>
     <row r="581">
-      <c r="D581" s="15"/>
+      <c r="D581" s="19"/>
     </row>
     <row r="582">
-      <c r="D582" s="15"/>
+      <c r="D582" s="19"/>
     </row>
     <row r="583">
-      <c r="D583" s="15"/>
+      <c r="D583" s="19"/>
     </row>
     <row r="584">
-      <c r="D584" s="15"/>
+      <c r="D584" s="19"/>
     </row>
     <row r="585">
-      <c r="D585" s="15"/>
+      <c r="D585" s="19"/>
     </row>
     <row r="586">
-      <c r="D586" s="15"/>
+      <c r="D586" s="19"/>
     </row>
     <row r="587">
-      <c r="D587" s="15"/>
+      <c r="D587" s="19"/>
     </row>
     <row r="588">
-      <c r="D588" s="15"/>
+      <c r="D588" s="19"/>
     </row>
     <row r="589">
-      <c r="D589" s="15"/>
+      <c r="D589" s="19"/>
     </row>
     <row r="590">
-      <c r="D590" s="15"/>
+      <c r="D590" s="19"/>
     </row>
     <row r="591">
-      <c r="D591" s="15"/>
+      <c r="D591" s="19"/>
     </row>
     <row r="592">
-      <c r="D592" s="15"/>
+      <c r="D592" s="19"/>
     </row>
     <row r="593">
-      <c r="D593" s="15"/>
+      <c r="D593" s="19"/>
     </row>
     <row r="594">
-      <c r="D594" s="15"/>
+      <c r="D594" s="19"/>
     </row>
     <row r="595">
-      <c r="D595" s="15"/>
+      <c r="D595" s="19"/>
     </row>
     <row r="596">
-      <c r="D596" s="15"/>
+      <c r="D596" s="19"/>
     </row>
     <row r="597">
-      <c r="D597" s="15"/>
+      <c r="D597" s="19"/>
     </row>
     <row r="598">
-      <c r="D598" s="15"/>
+      <c r="D598" s="19"/>
     </row>
     <row r="599">
-      <c r="D599" s="15"/>
+      <c r="D599" s="19"/>
     </row>
     <row r="600">
-      <c r="D600" s="15"/>
+      <c r="D600" s="19"/>
     </row>
     <row r="601">
-      <c r="D601" s="15"/>
+      <c r="D601" s="19"/>
     </row>
     <row r="602">
-      <c r="D602" s="15"/>
+      <c r="D602" s="19"/>
     </row>
     <row r="603">
-      <c r="D603" s="15"/>
+      <c r="D603" s="19"/>
     </row>
     <row r="604">
-      <c r="D604" s="15"/>
+      <c r="D604" s="19"/>
     </row>
     <row r="605">
-      <c r="D605" s="15"/>
+      <c r="D605" s="19"/>
     </row>
     <row r="606">
-      <c r="D606" s="15"/>
+      <c r="D606" s="19"/>
     </row>
     <row r="607">
-      <c r="D607" s="15"/>
+      <c r="D607" s="19"/>
     </row>
     <row r="608">
-      <c r="D608" s="15"/>
+      <c r="D608" s="19"/>
     </row>
     <row r="609">
-      <c r="D609" s="15"/>
+      <c r="D609" s="19"/>
     </row>
     <row r="610">
-      <c r="D610" s="15"/>
+      <c r="D610" s="19"/>
     </row>
     <row r="611">
-      <c r="D611" s="15"/>
+      <c r="D611" s="19"/>
     </row>
     <row r="612">
-      <c r="D612" s="15"/>
+      <c r="D612" s="19"/>
     </row>
     <row r="613">
-      <c r="D613" s="15"/>
+      <c r="D613" s="19"/>
     </row>
     <row r="614">
-      <c r="D614" s="15"/>
+      <c r="D614" s="19"/>
     </row>
     <row r="615">
-      <c r="D615" s="15"/>
+      <c r="D615" s="19"/>
     </row>
     <row r="616">
-      <c r="D616" s="15"/>
+      <c r="D616" s="19"/>
     </row>
     <row r="617">
-      <c r="D617" s="15"/>
+      <c r="D617" s="19"/>
     </row>
     <row r="618">
-      <c r="D618" s="15"/>
+      <c r="D618" s="19"/>
     </row>
     <row r="619">
-      <c r="D619" s="15"/>
+      <c r="D619" s="19"/>
     </row>
     <row r="620">
-      <c r="D620" s="15"/>
+      <c r="D620" s="19"/>
     </row>
     <row r="621">
-      <c r="D621" s="15"/>
+      <c r="D621" s="19"/>
     </row>
     <row r="622">
-      <c r="D622" s="15"/>
+      <c r="D622" s="19"/>
     </row>
     <row r="623">
-      <c r="D623" s="15"/>
+      <c r="D623" s="19"/>
     </row>
     <row r="624">
-      <c r="D624" s="15"/>
+      <c r="D624" s="19"/>
     </row>
     <row r="625">
-      <c r="D625" s="15"/>
+      <c r="D625" s="19"/>
     </row>
     <row r="626">
-      <c r="D626" s="15"/>
+      <c r="D626" s="19"/>
     </row>
     <row r="627">
-      <c r="D627" s="15"/>
+      <c r="D627" s="19"/>
     </row>
     <row r="628">
-      <c r="D628" s="15"/>
+      <c r="D628" s="19"/>
     </row>
     <row r="629">
-      <c r="D629" s="15"/>
+      <c r="D629" s="19"/>
     </row>
     <row r="630">
-      <c r="D630" s="15"/>
+      <c r="D630" s="19"/>
     </row>
     <row r="631">
-      <c r="D631" s="15"/>
+      <c r="D631" s="19"/>
     </row>
     <row r="632">
-      <c r="D632" s="15"/>
+      <c r="D632" s="19"/>
     </row>
     <row r="633">
-      <c r="D633" s="15"/>
+      <c r="D633" s="19"/>
     </row>
     <row r="634">
-      <c r="D634" s="15"/>
+      <c r="D634" s="19"/>
     </row>
     <row r="635">
-      <c r="D635" s="15"/>
+      <c r="D635" s="19"/>
     </row>
     <row r="636">
-      <c r="D636" s="15"/>
+      <c r="D636" s="19"/>
     </row>
     <row r="637">
-      <c r="D637" s="15"/>
+      <c r="D637" s="19"/>
     </row>
     <row r="638">
-      <c r="D638" s="15"/>
+      <c r="D638" s="19"/>
     </row>
     <row r="639">
-      <c r="D639" s="15"/>
+      <c r="D639" s="19"/>
     </row>
     <row r="640">
-      <c r="D640" s="15"/>
+      <c r="D640" s="19"/>
     </row>
     <row r="641">
-      <c r="D641" s="15"/>
+      <c r="D641" s="19"/>
     </row>
     <row r="642">
-      <c r="D642" s="15"/>
+      <c r="D642" s="19"/>
     </row>
     <row r="643">
-      <c r="D643" s="15"/>
+      <c r="D643" s="19"/>
     </row>
     <row r="644">
-      <c r="D644" s="15"/>
+      <c r="D644" s="19"/>
     </row>
     <row r="645">
-      <c r="D645" s="15"/>
+      <c r="D645" s="19"/>
     </row>
     <row r="646">
-      <c r="D646" s="15"/>
+      <c r="D646" s="19"/>
     </row>
     <row r="647">
-      <c r="D647" s="15"/>
+      <c r="D647" s="19"/>
     </row>
     <row r="648">
-      <c r="D648" s="15"/>
+      <c r="D648" s="19"/>
     </row>
     <row r="649">
-      <c r="D649" s="15"/>
+      <c r="D649" s="19"/>
     </row>
     <row r="650">
-      <c r="D650" s="15"/>
+      <c r="D650" s="19"/>
     </row>
     <row r="651">
-      <c r="D651" s="15"/>
+      <c r="D651" s="19"/>
     </row>
     <row r="652">
-      <c r="D652" s="15"/>
+      <c r="D652" s="19"/>
     </row>
     <row r="653">
-      <c r="D653" s="15"/>
+      <c r="D653" s="19"/>
     </row>
     <row r="654">
-      <c r="D654" s="15"/>
+      <c r="D654" s="19"/>
     </row>
     <row r="655">
-      <c r="D655" s="15"/>
+      <c r="D655" s="19"/>
     </row>
     <row r="656">
-      <c r="D656" s="15"/>
+      <c r="D656" s="19"/>
     </row>
     <row r="657">
-      <c r="D657" s="15"/>
+      <c r="D657" s="19"/>
     </row>
     <row r="658">
-      <c r="D658" s="15"/>
+      <c r="D658" s="19"/>
     </row>
     <row r="659">
-      <c r="D659" s="15"/>
+      <c r="D659" s="19"/>
     </row>
     <row r="660">
-      <c r="D660" s="15"/>
+      <c r="D660" s="19"/>
     </row>
     <row r="661">
-      <c r="D661" s="15"/>
+      <c r="D661" s="19"/>
     </row>
     <row r="662">
-      <c r="D662" s="15"/>
+      <c r="D662" s="19"/>
     </row>
     <row r="663">
-      <c r="D663" s="15"/>
+      <c r="D663" s="19"/>
     </row>
     <row r="664">
-      <c r="D664" s="15"/>
+      <c r="D664" s="19"/>
     </row>
     <row r="665">
-      <c r="D665" s="15"/>
+      <c r="D665" s="19"/>
     </row>
     <row r="666">
-      <c r="D666" s="15"/>
+      <c r="D666" s="19"/>
     </row>
     <row r="667">
-      <c r="D667" s="15"/>
+      <c r="D667" s="19"/>
     </row>
     <row r="668">
-      <c r="D668" s="15"/>
+      <c r="D668" s="19"/>
     </row>
     <row r="669">
-      <c r="D669" s="15"/>
+      <c r="D669" s="19"/>
     </row>
     <row r="670">
-      <c r="D670" s="15"/>
+      <c r="D670" s="19"/>
     </row>
     <row r="671">
-      <c r="D671" s="15"/>
+      <c r="D671" s="19"/>
     </row>
     <row r="672">
-      <c r="D672" s="15"/>
+      <c r="D672" s="19"/>
     </row>
     <row r="673">
-      <c r="D673" s="15"/>
+      <c r="D673" s="19"/>
     </row>
     <row r="674">
-      <c r="D674" s="15"/>
+      <c r="D674" s="19"/>
     </row>
     <row r="675">
-      <c r="D675" s="15"/>
+      <c r="D675" s="19"/>
     </row>
     <row r="676">
-      <c r="D676" s="15"/>
+      <c r="D676" s="19"/>
     </row>
     <row r="677">
-      <c r="D677" s="15"/>
+      <c r="D677" s="19"/>
     </row>
     <row r="678">
-      <c r="D678" s="15"/>
+      <c r="D678" s="19"/>
     </row>
     <row r="679">
-      <c r="D679" s="15"/>
+      <c r="D679" s="19"/>
     </row>
     <row r="680">
-      <c r="D680" s="15"/>
+      <c r="D680" s="19"/>
     </row>
     <row r="681">
-      <c r="D681" s="15"/>
+      <c r="D681" s="19"/>
     </row>
     <row r="682">
-      <c r="D682" s="15"/>
+      <c r="D682" s="19"/>
     </row>
     <row r="683">
-      <c r="D683" s="15"/>
+      <c r="D683" s="19"/>
     </row>
     <row r="684">
-      <c r="D684" s="15"/>
+      <c r="D684" s="19"/>
     </row>
     <row r="685">
-      <c r="D685" s="15"/>
+      <c r="D685" s="19"/>
     </row>
     <row r="686">
-      <c r="D686" s="15"/>
+      <c r="D686" s="19"/>
     </row>
     <row r="687">
-      <c r="D687" s="15"/>
+      <c r="D687" s="19"/>
     </row>
     <row r="688">
-      <c r="D688" s="15"/>
+      <c r="D688" s="19"/>
     </row>
     <row r="689">
-      <c r="D689" s="15"/>
+      <c r="D689" s="19"/>
     </row>
     <row r="690">
-      <c r="D690" s="15"/>
+      <c r="D690" s="19"/>
     </row>
     <row r="691">
-      <c r="D691" s="15"/>
+      <c r="D691" s="19"/>
     </row>
     <row r="692">
-      <c r="D692" s="15"/>
+      <c r="D692" s="19"/>
     </row>
     <row r="693">
-      <c r="D693" s="15"/>
+      <c r="D693" s="19"/>
     </row>
     <row r="694">
-      <c r="D694" s="15"/>
+      <c r="D694" s="19"/>
     </row>
     <row r="695">
-      <c r="D695" s="15"/>
+      <c r="D695" s="19"/>
     </row>
     <row r="696">
-      <c r="D696" s="15"/>
+      <c r="D696" s="19"/>
     </row>
     <row r="697">
-      <c r="D697" s="15"/>
+      <c r="D697" s="19"/>
     </row>
     <row r="698">
-      <c r="D698" s="15"/>
+      <c r="D698" s="19"/>
     </row>
     <row r="699">
-      <c r="D699" s="15"/>
+      <c r="D699" s="19"/>
     </row>
     <row r="700">
-      <c r="D700" s="15"/>
+      <c r="D700" s="19"/>
     </row>
     <row r="701">
-      <c r="D701" s="15"/>
+      <c r="D701" s="19"/>
     </row>
     <row r="702">
-      <c r="D702" s="15"/>
+      <c r="D702" s="19"/>
     </row>
     <row r="703">
-      <c r="D703" s="15"/>
+      <c r="D703" s="19"/>
     </row>
     <row r="704">
-      <c r="D704" s="15"/>
+      <c r="D704" s="19"/>
     </row>
     <row r="705">
-      <c r="D705" s="15"/>
+      <c r="D705" s="19"/>
     </row>
     <row r="706">
-      <c r="D706" s="15"/>
+      <c r="D706" s="19"/>
     </row>
     <row r="707">
-      <c r="D707" s="15"/>
+      <c r="D707" s="19"/>
     </row>
     <row r="708">
-      <c r="D708" s="15"/>
+      <c r="D708" s="19"/>
     </row>
     <row r="709">
-      <c r="D709" s="15"/>
+      <c r="D709" s="19"/>
     </row>
     <row r="710">
-      <c r="D710" s="15"/>
+      <c r="D710" s="19"/>
     </row>
     <row r="711">
-      <c r="D711" s="15"/>
+      <c r="D711" s="19"/>
     </row>
     <row r="712">
-      <c r="D712" s="15"/>
+      <c r="D712" s="19"/>
     </row>
     <row r="713">
-      <c r="D713" s="15"/>
+      <c r="D713" s="19"/>
     </row>
     <row r="714">
-      <c r="D714" s="15"/>
+      <c r="D714" s="19"/>
     </row>
     <row r="715">
-      <c r="D715" s="15"/>
+      <c r="D715" s="19"/>
     </row>
     <row r="716">
-      <c r="D716" s="15"/>
+      <c r="D716" s="19"/>
     </row>
     <row r="717">
-      <c r="D717" s="15"/>
+      <c r="D717" s="19"/>
     </row>
     <row r="718">
-      <c r="D718" s="15"/>
+      <c r="D718" s="19"/>
     </row>
     <row r="719">
-      <c r="D719" s="15"/>
+      <c r="D719" s="19"/>
     </row>
     <row r="720">
-      <c r="D720" s="15"/>
+      <c r="D720" s="19"/>
     </row>
     <row r="721">
-      <c r="D721" s="15"/>
+      <c r="D721" s="19"/>
     </row>
     <row r="722">
-      <c r="D722" s="15"/>
+      <c r="D722" s="19"/>
     </row>
     <row r="723">
-      <c r="D723" s="15"/>
+      <c r="D723" s="19"/>
     </row>
     <row r="724">
-      <c r="D724" s="15"/>
+      <c r="D724" s="19"/>
     </row>
     <row r="725">
-      <c r="D725" s="15"/>
+      <c r="D725" s="19"/>
     </row>
     <row r="726">
-      <c r="D726" s="15"/>
+      <c r="D726" s="19"/>
     </row>
     <row r="727">
-      <c r="D727" s="15"/>
+      <c r="D727" s="19"/>
     </row>
     <row r="728">
-      <c r="D728" s="15"/>
+      <c r="D728" s="19"/>
     </row>
     <row r="729">
-      <c r="D729" s="15"/>
+      <c r="D729" s="19"/>
     </row>
     <row r="730">
-      <c r="D730" s="15"/>
+      <c r="D730" s="19"/>
     </row>
     <row r="731">
-      <c r="D731" s="15"/>
+      <c r="D731" s="19"/>
     </row>
     <row r="732">
-      <c r="D732" s="15"/>
+      <c r="D732" s="19"/>
     </row>
     <row r="733">
-      <c r="D733" s="15"/>
+      <c r="D733" s="19"/>
     </row>
     <row r="734">
-      <c r="D734" s="15"/>
+      <c r="D734" s="19"/>
     </row>
     <row r="735">
-      <c r="D735" s="15"/>
+      <c r="D735" s="19"/>
     </row>
     <row r="736">
-      <c r="D736" s="15"/>
+      <c r="D736" s="19"/>
     </row>
     <row r="737">
-      <c r="D737" s="15"/>
+      <c r="D737" s="19"/>
     </row>
     <row r="738">
-      <c r="D738" s="15"/>
+      <c r="D738" s="19"/>
     </row>
     <row r="739">
-      <c r="D739" s="15"/>
+      <c r="D739" s="19"/>
     </row>
     <row r="740">
-      <c r="D740" s="15"/>
+      <c r="D740" s="19"/>
     </row>
     <row r="741">
-      <c r="D741" s="15"/>
+      <c r="D741" s="19"/>
     </row>
     <row r="742">
-      <c r="D742" s="15"/>
+      <c r="D742" s="19"/>
     </row>
     <row r="743">
-      <c r="D743" s="15"/>
+      <c r="D743" s="19"/>
     </row>
     <row r="744">
-      <c r="D744" s="15"/>
+      <c r="D744" s="19"/>
     </row>
     <row r="745">
-      <c r="D745" s="15"/>
+      <c r="D745" s="19"/>
     </row>
     <row r="746">
-      <c r="D746" s="15"/>
+      <c r="D746" s="19"/>
     </row>
     <row r="747">
-      <c r="D747" s="15"/>
+      <c r="D747" s="19"/>
     </row>
     <row r="748">
-      <c r="D748" s="15"/>
+      <c r="D748" s="19"/>
     </row>
     <row r="749">
-      <c r="D749" s="15"/>
+      <c r="D749" s="19"/>
     </row>
     <row r="750">
-      <c r="D750" s="15"/>
+      <c r="D750" s="19"/>
     </row>
     <row r="751">
-      <c r="D751" s="15"/>
+      <c r="D751" s="19"/>
     </row>
     <row r="752">
-      <c r="D752" s="15"/>
+      <c r="D752" s="19"/>
     </row>
     <row r="753">
-      <c r="D753" s="15"/>
+      <c r="D753" s="19"/>
     </row>
     <row r="754">
-      <c r="D754" s="15"/>
+      <c r="D754" s="19"/>
     </row>
     <row r="755">
-      <c r="D755" s="15"/>
+      <c r="D755" s="19"/>
     </row>
     <row r="756">
-      <c r="D756" s="15"/>
+      <c r="D756" s="19"/>
     </row>
     <row r="757">
-      <c r="D757" s="15"/>
+      <c r="D757" s="19"/>
     </row>
     <row r="758">
-      <c r="D758" s="15"/>
+      <c r="D758" s="19"/>
     </row>
     <row r="759">
-      <c r="D759" s="15"/>
+      <c r="D759" s="19"/>
     </row>
     <row r="760">
-      <c r="D760" s="15"/>
+      <c r="D760" s="19"/>
     </row>
     <row r="761">
-      <c r="D761" s="15"/>
+      <c r="D761" s="19"/>
     </row>
     <row r="762">
-      <c r="D762" s="15"/>
+      <c r="D762" s="19"/>
     </row>
     <row r="763">
-      <c r="D763" s="15"/>
+      <c r="D763" s="19"/>
     </row>
     <row r="764">
-      <c r="D764" s="15"/>
+      <c r="D764" s="19"/>
     </row>
     <row r="765">
-      <c r="D765" s="15"/>
+      <c r="D765" s="19"/>
     </row>
     <row r="766">
-      <c r="D766" s="15"/>
+      <c r="D766" s="19"/>
     </row>
     <row r="767">
-      <c r="D767" s="15"/>
+      <c r="D767" s="19"/>
     </row>
     <row r="768">
-      <c r="D768" s="15"/>
+      <c r="D768" s="19"/>
     </row>
     <row r="769">
-      <c r="D769" s="15"/>
+      <c r="D769" s="19"/>
     </row>
     <row r="770">
-      <c r="D770" s="15"/>
+      <c r="D770" s="19"/>
     </row>
     <row r="771">
-      <c r="D771" s="15"/>
+      <c r="D771" s="19"/>
     </row>
     <row r="772">
-      <c r="D772" s="15"/>
+      <c r="D772" s="19"/>
     </row>
     <row r="773">
-      <c r="D773" s="15"/>
+      <c r="D773" s="19"/>
     </row>
     <row r="774">
-      <c r="D774" s="15"/>
+      <c r="D774" s="19"/>
     </row>
     <row r="775">
-      <c r="D775" s="15"/>
+      <c r="D775" s="19"/>
     </row>
     <row r="776">
-      <c r="D776" s="15"/>
+      <c r="D776" s="19"/>
     </row>
     <row r="777">
-      <c r="D777" s="15"/>
+      <c r="D777" s="19"/>
     </row>
     <row r="778">
-      <c r="D778" s="15"/>
+      <c r="D778" s="19"/>
     </row>
     <row r="779">
-      <c r="D779" s="15"/>
+      <c r="D779" s="19"/>
     </row>
     <row r="780">
-      <c r="D780" s="15"/>
+      <c r="D780" s="19"/>
     </row>
     <row r="781">
-      <c r="D781" s="15"/>
+      <c r="D781" s="19"/>
     </row>
     <row r="782">
-      <c r="D782" s="15"/>
+      <c r="D782" s="19"/>
     </row>
     <row r="783">
-      <c r="D783" s="15"/>
+      <c r="D783" s="19"/>
     </row>
     <row r="784">
-      <c r="D784" s="15"/>
+      <c r="D784" s="19"/>
     </row>
     <row r="785">
-      <c r="D785" s="15"/>
+      <c r="D785" s="19"/>
     </row>
     <row r="786">
-      <c r="D786" s="15"/>
+      <c r="D786" s="19"/>
     </row>
     <row r="787">
-      <c r="D787" s="15"/>
+      <c r="D787" s="19"/>
     </row>
     <row r="788">
-      <c r="D788" s="15"/>
+      <c r="D788" s="19"/>
     </row>
     <row r="789">
-      <c r="D789" s="15"/>
+      <c r="D789" s="19"/>
     </row>
     <row r="790">
-      <c r="D790" s="15"/>
+      <c r="D790" s="19"/>
     </row>
     <row r="791">
-      <c r="D791" s="15"/>
+      <c r="D791" s="19"/>
     </row>
     <row r="792">
-      <c r="D792" s="15"/>
+      <c r="D792" s="19"/>
     </row>
     <row r="793">
-      <c r="D793" s="15"/>
+      <c r="D793" s="19"/>
     </row>
     <row r="794">
-      <c r="D794" s="15"/>
+      <c r="D794" s="19"/>
     </row>
     <row r="795">
-      <c r="D795" s="15"/>
+      <c r="D795" s="19"/>
     </row>
     <row r="796">
-      <c r="D796" s="15"/>
+      <c r="D796" s="19"/>
     </row>
     <row r="797">
-      <c r="D797" s="15"/>
+      <c r="D797" s="19"/>
     </row>
     <row r="798">
-      <c r="D798" s="15"/>
+      <c r="D798" s="19"/>
     </row>
     <row r="799">
-      <c r="D799" s="15"/>
+      <c r="D799" s="19"/>
     </row>
     <row r="800">
-      <c r="D800" s="15"/>
+      <c r="D800" s="19"/>
     </row>
     <row r="801">
-      <c r="D801" s="15"/>
+      <c r="D801" s="19"/>
     </row>
     <row r="802">
-      <c r="D802" s="15"/>
+      <c r="D802" s="19"/>
     </row>
     <row r="803">
-      <c r="D803" s="15"/>
+      <c r="D803" s="19"/>
     </row>
     <row r="804">
-      <c r="D804" s="15"/>
+      <c r="D804" s="19"/>
     </row>
     <row r="805">
-      <c r="D805" s="15"/>
+      <c r="D805" s="19"/>
     </row>
     <row r="806">
-      <c r="D806" s="15"/>
+      <c r="D806" s="19"/>
     </row>
     <row r="807">
-      <c r="D807" s="15"/>
+      <c r="D807" s="19"/>
     </row>
     <row r="808">
-      <c r="D808" s="15"/>
+      <c r="D808" s="19"/>
     </row>
     <row r="809">
-      <c r="D809" s="15"/>
+      <c r="D809" s="19"/>
     </row>
     <row r="810">
-      <c r="D810" s="15"/>
+      <c r="D810" s="19"/>
     </row>
     <row r="811">
-      <c r="D811" s="15"/>
+      <c r="D811" s="19"/>
     </row>
     <row r="812">
-      <c r="D812" s="15"/>
+      <c r="D812" s="19"/>
     </row>
     <row r="813">
-      <c r="D813" s="15"/>
+      <c r="D813" s="19"/>
     </row>
     <row r="814">
-      <c r="D814" s="15"/>
+      <c r="D814" s="19"/>
     </row>
     <row r="815">
-      <c r="D815" s="15"/>
+      <c r="D815" s="19"/>
     </row>
     <row r="816">
-      <c r="D816" s="15"/>
+      <c r="D816" s="19"/>
     </row>
     <row r="817">
-      <c r="D817" s="15"/>
+      <c r="D817" s="19"/>
     </row>
     <row r="818">
-      <c r="D818" s="15"/>
+      <c r="D818" s="19"/>
     </row>
     <row r="819">
-      <c r="D819" s="15"/>
+      <c r="D819" s="19"/>
     </row>
     <row r="820">
-      <c r="D820" s="15"/>
+      <c r="D820" s="19"/>
     </row>
     <row r="821">
-      <c r="D821" s="15"/>
+      <c r="D821" s="19"/>
     </row>
     <row r="822">
-      <c r="D822" s="15"/>
+      <c r="D822" s="19"/>
     </row>
     <row r="823">
-      <c r="D823" s="15"/>
+      <c r="D823" s="19"/>
     </row>
     <row r="824">
-      <c r="D824" s="15"/>
+      <c r="D824" s="19"/>
     </row>
     <row r="825">
-      <c r="D825" s="15"/>
+      <c r="D825" s="19"/>
     </row>
     <row r="826">
-      <c r="D826" s="15"/>
+      <c r="D826" s="19"/>
     </row>
     <row r="827">
-      <c r="D827" s="15"/>
+      <c r="D827" s="19"/>
     </row>
     <row r="828">
-      <c r="D828" s="15"/>
+      <c r="D828" s="19"/>
     </row>
     <row r="829">
-      <c r="D829" s="15"/>
+      <c r="D829" s="19"/>
     </row>
     <row r="830">
-      <c r="D830" s="15"/>
+      <c r="D830" s="19"/>
     </row>
     <row r="831">
-      <c r="D831" s="15"/>
+      <c r="D831" s="19"/>
     </row>
     <row r="832">
-      <c r="D832" s="15"/>
+      <c r="D832" s="19"/>
     </row>
     <row r="833">
-      <c r="D833" s="15"/>
+      <c r="D833" s="19"/>
     </row>
     <row r="834">
-      <c r="D834" s="15"/>
+      <c r="D834" s="19"/>
     </row>
     <row r="835">
-      <c r="D835" s="15"/>
+      <c r="D835" s="19"/>
     </row>
     <row r="836">
-      <c r="D836" s="15"/>
+      <c r="D836" s="19"/>
     </row>
     <row r="837">
-      <c r="D837" s="15"/>
+      <c r="D837" s="19"/>
     </row>
     <row r="838">
-      <c r="D838" s="15"/>
+      <c r="D838" s="19"/>
     </row>
     <row r="839">
-      <c r="D839" s="15"/>
+      <c r="D839" s="19"/>
     </row>
     <row r="840">
-      <c r="D840" s="15"/>
+      <c r="D840" s="19"/>
     </row>
     <row r="841">
-      <c r="D841" s="15"/>
+      <c r="D841" s="19"/>
     </row>
     <row r="842">
-      <c r="D842" s="15"/>
+      <c r="D842" s="19"/>
     </row>
     <row r="843">
-      <c r="D843" s="15"/>
+      <c r="D843" s="19"/>
     </row>
     <row r="844">
-      <c r="D844" s="15"/>
+      <c r="D844" s="19"/>
     </row>
     <row r="845">
-      <c r="D845" s="15"/>
+      <c r="D845" s="19"/>
     </row>
     <row r="846">
-      <c r="D846" s="15"/>
+      <c r="D846" s="19"/>
     </row>
     <row r="847">
-      <c r="D847" s="15"/>
+      <c r="D847" s="19"/>
     </row>
     <row r="848">
-      <c r="D848" s="15"/>
+      <c r="D848" s="19"/>
     </row>
     <row r="849">
-      <c r="D849" s="15"/>
+      <c r="D849" s="19"/>
     </row>
     <row r="850">
-      <c r="D850" s="15"/>
+      <c r="D850" s="19"/>
     </row>
     <row r="851">
-      <c r="D851" s="15"/>
+      <c r="D851" s="19"/>
     </row>
     <row r="852">
-      <c r="D852" s="15"/>
+      <c r="D852" s="19"/>
     </row>
     <row r="853">
-      <c r="D853" s="15"/>
+      <c r="D853" s="19"/>
     </row>
     <row r="854">
-      <c r="D854" s="15"/>
+      <c r="D854" s="19"/>
     </row>
     <row r="855">
-      <c r="D855" s="15"/>
+      <c r="D855" s="19"/>
     </row>
     <row r="856">
-      <c r="D856" s="15"/>
+      <c r="D856" s="19"/>
     </row>
     <row r="857">
-      <c r="D857" s="15"/>
+      <c r="D857" s="19"/>
     </row>
     <row r="858">
-      <c r="D858" s="15"/>
+      <c r="D858" s="19"/>
     </row>
     <row r="859">
-      <c r="D859" s="15"/>
+      <c r="D859" s="19"/>
     </row>
     <row r="860">
-      <c r="D860" s="15"/>
+      <c r="D860" s="19"/>
     </row>
     <row r="861">
-      <c r="D861" s="15"/>
+      <c r="D861" s="19"/>
     </row>
     <row r="862">
-      <c r="D862" s="15"/>
+      <c r="D862" s="19"/>
     </row>
     <row r="863">
-      <c r="D863" s="15"/>
+      <c r="D863" s="19"/>
     </row>
     <row r="864">
-      <c r="D864" s="15"/>
+      <c r="D864" s="19"/>
     </row>
     <row r="865">
-      <c r="D865" s="15"/>
+      <c r="D865" s="19"/>
     </row>
     <row r="866">
-      <c r="D866" s="15"/>
+      <c r="D866" s="19"/>
     </row>
     <row r="867">
-      <c r="D867" s="15"/>
+      <c r="D867" s="19"/>
     </row>
     <row r="868">
-      <c r="D868" s="15"/>
+      <c r="D868" s="19"/>
     </row>
     <row r="869">
-      <c r="D869" s="15"/>
+      <c r="D869" s="19"/>
     </row>
     <row r="870">
-      <c r="D870" s="15"/>
+      <c r="D870" s="19"/>
     </row>
     <row r="871">
-      <c r="D871" s="15"/>
+      <c r="D871" s="19"/>
     </row>
     <row r="872">
-      <c r="D872" s="15"/>
+      <c r="D872" s="19"/>
     </row>
     <row r="873">
-      <c r="D873" s="15"/>
+      <c r="D873" s="19"/>
     </row>
     <row r="874">
-      <c r="D874" s="15"/>
+      <c r="D874" s="19"/>
     </row>
     <row r="875">
-      <c r="D875" s="15"/>
+      <c r="D875" s="19"/>
     </row>
     <row r="876">
-      <c r="D876" s="15"/>
+      <c r="D876" s="19"/>
     </row>
     <row r="877">
-      <c r="D877" s="15"/>
+      <c r="D877" s="19"/>
     </row>
     <row r="878">
-      <c r="D878" s="15"/>
+      <c r="D878" s="19"/>
     </row>
     <row r="879">
-      <c r="D879" s="15"/>
+      <c r="D879" s="19"/>
     </row>
     <row r="880">
-      <c r="D880" s="15"/>
+      <c r="D880" s="19"/>
     </row>
     <row r="881">
-      <c r="D881" s="15"/>
+      <c r="D881" s="19"/>
     </row>
     <row r="882">
-      <c r="D882" s="15"/>
+      <c r="D882" s="19"/>
     </row>
     <row r="883">
-      <c r="D883" s="15"/>
+      <c r="D883" s="19"/>
     </row>
     <row r="884">
-      <c r="D884" s="15"/>
+      <c r="D884" s="19"/>
     </row>
     <row r="885">
-      <c r="D885" s="15"/>
+      <c r="D885" s="19"/>
     </row>
     <row r="886">
-      <c r="D886" s="15"/>
+      <c r="D886" s="19"/>
     </row>
     <row r="887">
-      <c r="D887" s="15"/>
+      <c r="D887" s="19"/>
     </row>
     <row r="888">
-      <c r="D888" s="15"/>
+      <c r="D888" s="19"/>
     </row>
     <row r="889">
-      <c r="D889" s="15"/>
+      <c r="D889" s="19"/>
     </row>
     <row r="890">
-      <c r="D890" s="15"/>
+      <c r="D890" s="19"/>
     </row>
     <row r="891">
-      <c r="D891" s="15"/>
+      <c r="D891" s="19"/>
     </row>
     <row r="892">
-      <c r="D892" s="15"/>
+      <c r="D892" s="19"/>
     </row>
     <row r="893">
-      <c r="D893" s="15"/>
+      <c r="D893" s="19"/>
     </row>
     <row r="894">
-      <c r="D894" s="15"/>
+      <c r="D894" s="19"/>
     </row>
     <row r="895">
-      <c r="D895" s="15"/>
+      <c r="D895" s="19"/>
     </row>
     <row r="896">
-      <c r="D896" s="15"/>
+      <c r="D896" s="19"/>
     </row>
     <row r="897">
-      <c r="D897" s="15"/>
+      <c r="D897" s="19"/>
     </row>
     <row r="898">
-      <c r="D898" s="15"/>
+      <c r="D898" s="19"/>
     </row>
     <row r="899">
-      <c r="D899" s="15"/>
+      <c r="D899" s="19"/>
     </row>
     <row r="900">
-      <c r="D900" s="15"/>
+      <c r="D900" s="19"/>
     </row>
     <row r="901">
-      <c r="D901" s="15"/>
+      <c r="D901" s="19"/>
     </row>
     <row r="902">
-      <c r="D902" s="15"/>
+      <c r="D902" s="19"/>
     </row>
     <row r="903">
-      <c r="D903" s="15"/>
+      <c r="D903" s="19"/>
     </row>
     <row r="904">
-      <c r="D904" s="15"/>
+      <c r="D904" s="19"/>
     </row>
     <row r="905">
-      <c r="D905" s="15"/>
+      <c r="D905" s="19"/>
     </row>
     <row r="906">
-      <c r="D906" s="15"/>
+      <c r="D906" s="19"/>
     </row>
     <row r="907">
-      <c r="D907" s="15"/>
+      <c r="D907" s="19"/>
     </row>
     <row r="908">
-      <c r="D908" s="15"/>
+      <c r="D908" s="19"/>
     </row>
     <row r="909">
-      <c r="D909" s="15"/>
+      <c r="D909" s="19"/>
     </row>
     <row r="910">
-      <c r="D910" s="15"/>
+      <c r="D910" s="19"/>
     </row>
     <row r="911">
-      <c r="D911" s="15"/>
+      <c r="D911" s="19"/>
     </row>
     <row r="912">
-      <c r="D912" s="15"/>
+      <c r="D912" s="19"/>
     </row>
     <row r="913">
-      <c r="D913" s="15"/>
+      <c r="D913" s="19"/>
     </row>
     <row r="914">
-      <c r="D914" s="15"/>
+      <c r="D914" s="19"/>
     </row>
     <row r="915">
-      <c r="D915" s="15"/>
+      <c r="D915" s="19"/>
     </row>
     <row r="916">
-      <c r="D916" s="15"/>
+      <c r="D916" s="19"/>
     </row>
     <row r="917">
-      <c r="D917" s="15"/>
+      <c r="D917" s="19"/>
     </row>
     <row r="918">
-      <c r="D918" s="15"/>
+      <c r="D918" s="19"/>
     </row>
     <row r="919">
-      <c r="D919" s="15"/>
+      <c r="D919" s="19"/>
     </row>
     <row r="920">
-      <c r="D920" s="15"/>
+      <c r="D920" s="19"/>
     </row>
     <row r="921">
-      <c r="D921" s="15"/>
+      <c r="D921" s="19"/>
     </row>
     <row r="922">
-      <c r="D922" s="15"/>
+      <c r="D922" s="19"/>
     </row>
     <row r="923">
-      <c r="D923" s="15"/>
+      <c r="D923" s="19"/>
     </row>
     <row r="924">
-      <c r="D924" s="15"/>
+      <c r="D924" s="19"/>
     </row>
     <row r="925">
-      <c r="D925" s="15"/>
+      <c r="D925" s="19"/>
     </row>
     <row r="926">
-      <c r="D926" s="15"/>
+      <c r="D926" s="19"/>
     </row>
     <row r="927">
-      <c r="D927" s="15"/>
+      <c r="D927" s="19"/>
     </row>
     <row r="928">
-      <c r="D928" s="15"/>
+      <c r="D928" s="19"/>
     </row>
     <row r="929">
-      <c r="D929" s="15"/>
+      <c r="D929" s="19"/>
     </row>
     <row r="930">
-      <c r="D930" s="15"/>
+      <c r="D930" s="19"/>
     </row>
     <row r="931">
-      <c r="D931" s="15"/>
+      <c r="D931" s="19"/>
     </row>
     <row r="932">
-      <c r="D932" s="15"/>
+      <c r="D932" s="19"/>
     </row>
     <row r="933">
-      <c r="D933" s="15"/>
+      <c r="D933" s="19"/>
     </row>
     <row r="934">
-      <c r="D934" s="15"/>
+      <c r="D934" s="19"/>
     </row>
     <row r="935">
-      <c r="D935" s="15"/>
+      <c r="D935" s="19"/>
     </row>
     <row r="936">
-      <c r="D936" s="15"/>
+      <c r="D936" s="19"/>
     </row>
     <row r="937">
-      <c r="D937" s="15"/>
+      <c r="D937" s="19"/>
     </row>
     <row r="938">
-      <c r="D938" s="15"/>
+      <c r="D938" s="19"/>
     </row>
     <row r="939">
-      <c r="D939" s="15"/>
+      <c r="D939" s="19"/>
     </row>
     <row r="940">
-      <c r="D940" s="15"/>
+      <c r="D940" s="19"/>
     </row>
     <row r="941">
-      <c r="D941" s="15"/>
+      <c r="D941" s="19"/>
     </row>
     <row r="942">
-      <c r="D942" s="15"/>
+      <c r="D942" s="19"/>
     </row>
     <row r="943">
-      <c r="D943" s="15"/>
+      <c r="D943" s="19"/>
     </row>
     <row r="944">
-      <c r="D944" s="15"/>
+      <c r="D944" s="19"/>
     </row>
     <row r="945">
-      <c r="D945" s="15"/>
+      <c r="D945" s="19"/>
     </row>
     <row r="946">
-      <c r="D946" s="15"/>
+      <c r="D946" s="19"/>
     </row>
     <row r="947">
-      <c r="D947" s="15"/>
+      <c r="D947" s="19"/>
     </row>
     <row r="948">
-      <c r="D948" s="15"/>
+      <c r="D948" s="19"/>
     </row>
     <row r="949">
-      <c r="D949" s="15"/>
+      <c r="D949" s="19"/>
     </row>
     <row r="950">
-      <c r="D950" s="15"/>
+      <c r="D950" s="19"/>
     </row>
     <row r="951">
-      <c r="D951" s="15"/>
+      <c r="D951" s="19"/>
     </row>
     <row r="952">
-      <c r="D952" s="15"/>
+      <c r="D952" s="19"/>
     </row>
     <row r="953">
-      <c r="D953" s="15"/>
+      <c r="D953" s="19"/>
     </row>
     <row r="954">
-      <c r="D954" s="15"/>
+      <c r="D954" s="19"/>
     </row>
     <row r="955">
-      <c r="D955" s="15"/>
+      <c r="D955" s="19"/>
     </row>
     <row r="956">
-      <c r="D956" s="15"/>
+      <c r="D956" s="19"/>
     </row>
     <row r="957">
-      <c r="D957" s="15"/>
+      <c r="D957" s="19"/>
     </row>
     <row r="958">
-      <c r="D958" s="15"/>
+      <c r="D958" s="19"/>
     </row>
     <row r="959">
-      <c r="D959" s="15"/>
+      <c r="D959" s="19"/>
     </row>
     <row r="960">
-      <c r="D960" s="15"/>
+      <c r="D960" s="19"/>
     </row>
     <row r="961">
-      <c r="D961" s="15"/>
+      <c r="D961" s="19"/>
     </row>
     <row r="962">
-      <c r="D962" s="15"/>
+      <c r="D962" s="19"/>
     </row>
     <row r="963">
-      <c r="D963" s="15"/>
+      <c r="D963" s="19"/>
     </row>
     <row r="964">
-      <c r="D964" s="15"/>
+      <c r="D964" s="19"/>
     </row>
     <row r="965">
-      <c r="D965" s="15"/>
+      <c r="D965" s="19"/>
     </row>
     <row r="966">
-      <c r="D966" s="15"/>
+      <c r="D966" s="19"/>
     </row>
     <row r="967">
-      <c r="D967" s="15"/>
+      <c r="D967" s="19"/>
     </row>
     <row r="968">
-      <c r="D968" s="15"/>
+      <c r="D968" s="19"/>
     </row>
     <row r="969">
-      <c r="D969" s="15"/>
+      <c r="D969" s="19"/>
     </row>
     <row r="970">
-      <c r="D970" s="15"/>
+      <c r="D970" s="19"/>
     </row>
     <row r="971">
-      <c r="D971" s="15"/>
+      <c r="D971" s="19"/>
     </row>
     <row r="972">
-      <c r="D972" s="15"/>
+      <c r="D972" s="19"/>
     </row>
     <row r="973">
-      <c r="D973" s="15"/>
+      <c r="D973" s="19"/>
     </row>
     <row r="974">
-      <c r="D974" s="15"/>
+      <c r="D974" s="19"/>
     </row>
     <row r="975">
-      <c r="D975" s="15"/>
+      <c r="D975" s="19"/>
     </row>
     <row r="976">
-      <c r="D976" s="15"/>
+      <c r="D976" s="19"/>
     </row>
     <row r="977">
-      <c r="D977" s="15"/>
+      <c r="D977" s="19"/>
     </row>
     <row r="978">
-      <c r="D978" s="15"/>
+      <c r="D978" s="19"/>
     </row>
     <row r="979">
-      <c r="D979" s="15"/>
+      <c r="D979" s="19"/>
     </row>
     <row r="980">
-      <c r="D980" s="15"/>
+      <c r="D980" s="19"/>
     </row>
     <row r="981">
-      <c r="D981" s="15"/>
+      <c r="D981" s="19"/>
     </row>
     <row r="982">
-      <c r="D982" s="15"/>
+      <c r="D982" s="19"/>
     </row>
     <row r="983">
-      <c r="D983" s="15"/>
+      <c r="D983" s="19"/>
     </row>
     <row r="984">
-      <c r="D984" s="15"/>
+      <c r="D984" s="19"/>
     </row>
     <row r="985">
-      <c r="D985" s="15"/>
+      <c r="D985" s="19"/>
     </row>
     <row r="986">
-      <c r="D986" s="15"/>
+      <c r="D986" s="19"/>
     </row>
     <row r="987">
-      <c r="D987" s="15"/>
+      <c r="D987" s="19"/>
     </row>
     <row r="988">
-      <c r="D988" s="15"/>
+      <c r="D988" s="19"/>
     </row>
     <row r="989">
-      <c r="D989" s="15"/>
+      <c r="D989" s="19"/>
     </row>
     <row r="990">
-      <c r="D990" s="15"/>
+      <c r="D990" s="19"/>
     </row>
     <row r="991">
-      <c r="D991" s="15"/>
+      <c r="D991" s="19"/>
     </row>
     <row r="992">
-      <c r="D992" s="15"/>
+      <c r="D992" s="19"/>
     </row>
     <row r="993">
-      <c r="D993" s="15"/>
+      <c r="D993" s="19"/>
     </row>
     <row r="994">
-      <c r="D994" s="15"/>
+      <c r="D994" s="19"/>
     </row>
     <row r="995">
-      <c r="D995" s="15"/>
+      <c r="D995" s="19"/>
     </row>
     <row r="996">
-      <c r="D996" s="15"/>
+      <c r="D996" s="19"/>
     </row>
     <row r="997">
-      <c r="D997" s="15"/>
+      <c r="D997" s="19"/>
     </row>
     <row r="998">
-      <c r="D998" s="15"/>
+      <c r="D998" s="19"/>
     </row>
     <row r="999">
-      <c r="D999" s="15"/>
+      <c r="D999" s="19"/>
     </row>
     <row r="1000">
-      <c r="D1000" s="15"/>
+      <c r="D1000" s="19"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>